<commit_message>
Wow - Constraints Implemented (IK 0.1)
I finally got cone constraints working, with sphere constraints. This is the IK Update 0.1 where I began implementing the IK System... ;)
</commit_message>
<xml_diff>
--- a/Management & Logging/Planning and Management/AgilePlanning.xlsx
+++ b/Management & Logging/Planning and Management/AgilePlanning.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="186">
   <si>
     <t>Task Name</t>
   </si>
@@ -334,6 +334,7 @@
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -342,6 +343,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Behaviour Editor</t>
@@ -356,6 +358,7 @@
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -364,6 +367,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Custom Regional Path finding</t>
@@ -378,6 +382,7 @@
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -386,6 +391,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Build upon dialogue system</t>
@@ -400,6 +406,7 @@
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -408,6 +415,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Designing the AI States and beginning proceduralised states</t>
@@ -422,6 +430,7 @@
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -430,6 +439,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Writing the complex + dynamic combat system.</t>
@@ -444,6 +454,7 @@
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -452,6 +463,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Realistic NPC (Friend)</t>
@@ -466,6 +478,7 @@
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -474,6 +487,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Writing the communication system what each hand signal means and how  your friend will react to each one.</t>
@@ -504,6 +518,7 @@
         <sz val="11"/>
         <color rgb="FF006100"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>KNOW for sure</t>
@@ -719,6 +734,43 @@
   </si>
   <si>
     <t>The player fallst through the ground, so you need to check and fix it…</t>
+  </si>
+  <si>
+    <t>Fix the player clipping through the ground</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=YixF6p7YVeU</t>
+  </si>
+  <si>
+    <t>Issues/Notes</t>
+  </si>
+  <si>
+    <t>The pivoting system is just proceudrally done for now, it isn't perfect but it's fine. It works for now, the next thing I have to do now is the IK System. I cannottt wait. FABRIK here we come.</t>
+  </si>
+  <si>
+    <t>The procedural part of this will come when we finish the IK system and things like pivoting can be done through curves and rotating the pelvis and transitioning and changing to backward walk etc..</t>
+  </si>
+  <si>
+    <t>The player snaps through the floor sometimes, so check if input is affecting the instantaneous velocity which is measured each frame</t>
+  </si>
+  <si>
+    <t>This is important to make sure that the player isn't using up too many resources, make sure you disable features on the update when they aren't being used etc…</t>
+  </si>
+  <si>
+    <t>The IK system needs to be very flexible, with an editor that can attach bones, etc. New menu's and using normals to rotate the feet and then lift up the feet. Nice.</t>
+  </si>
+  <si>
+    <t>Using the blend trees and offsets to allow you to grab onto ledges, new controller.</t>
+  </si>
+  <si>
+    <t>By the end of this section you need, a simple walking animation that is smooth with pivoting and foot ik implemented with FABRIK. It also needs to have a rudimentary ledge climbing system that can hold onto ledges and hoist yourself up. This also needs to be displayed in a video, of him climbing up a ledge.</t>
+  </si>
+  <si>
+    <t>The end of this section also requires - 
+An animation for all states, and independent of movement blending between states procedurally using curves. Learn about masks and seperating upper/Lower body movement.</t>
   </si>
 </sst>
 </file>
@@ -831,11 +883,13 @@
       <sz val="7"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -843,6 +897,7 @@
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -885,7 +940,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -990,8 +1045,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1307,8 +1367,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
@@ -1321,8 +1396,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1678,18 +1754,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="27" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Neutral" xfId="6" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Seperator" xfId="7"/>
     <cellStyle name="Style 1" xfId="1"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="28">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBFDDAB"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1727,31 +1835,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBFDDAB"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -1814,41 +1897,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C7:M253" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="C7:M253"/>
-  <tableColumns count="11">
-    <tableColumn id="1" name="REF TAG" dataDxfId="24"/>
-    <tableColumn id="2" name="Task Name" dataDxfId="23"/>
-    <tableColumn id="3" name="BT 0.1" dataDxfId="22"/>
-    <tableColumn id="4" name="BT 0.2" dataDxfId="21"/>
-    <tableColumn id="5" name="BT 0.3" dataDxfId="20"/>
-    <tableColumn id="6" name="Break Down Notes" dataDxfId="19"/>
-    <tableColumn id="11" name="Hours left" dataDxfId="18">
-      <calculatedColumnFormula>_xlfn.DAYS(TODAY(), L8)*24</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C7:N253" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="C7:N253"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="REF TAG" dataDxfId="25"/>
+    <tableColumn id="2" name="Task Name" dataDxfId="24"/>
+    <tableColumn id="3" name="BT 0.1" dataDxfId="23"/>
+    <tableColumn id="4" name="BT 0.2" dataDxfId="22"/>
+    <tableColumn id="5" name="BT 0.3" dataDxfId="21"/>
+    <tableColumn id="6" name="Break Down Notes" dataDxfId="20"/>
+    <tableColumn id="12" name="Issues/Notes" dataDxfId="0"/>
+    <tableColumn id="11" name="Hours left" dataDxfId="19">
+      <calculatedColumnFormula>_xlfn.DAYS(TODAY(), M8)*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Completion Hours" dataDxfId="17"/>
-    <tableColumn id="8" name="Current Progress" dataDxfId="16"/>
-    <tableColumn id="9" name="Expected Completion Date" dataDxfId="15"/>
-    <tableColumn id="10" name="Real Completion Date" dataDxfId="14"/>
+    <tableColumn id="7" name="Completion Hours" dataDxfId="18"/>
+    <tableColumn id="8" name="Current Progress" dataDxfId="17"/>
+    <tableColumn id="9" name="Expected Completion Date" dataDxfId="16"/>
+    <tableColumn id="10" name="Real Completion Date" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="C7:L233" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="C7:L233" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="C7:L233"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="REF TAG" dataDxfId="9"/>
-    <tableColumn id="2" name="Task Name" dataDxfId="8"/>
-    <tableColumn id="3" name="BT 0.1" dataDxfId="7"/>
-    <tableColumn id="4" name="BT 0.2" dataDxfId="6"/>
-    <tableColumn id="5" name="BT 0.3" dataDxfId="5"/>
-    <tableColumn id="6" name="Break Down Notes" dataDxfId="4"/>
-    <tableColumn id="7" name="Completion Hours" dataDxfId="3"/>
-    <tableColumn id="8" name="Current Progress" dataDxfId="2"/>
-    <tableColumn id="9" name="Expected Completion Date" dataDxfId="1"/>
-    <tableColumn id="10" name="Real Completion Date" dataDxfId="0"/>
+    <tableColumn id="1" name="REF TAG" dataDxfId="12"/>
+    <tableColumn id="2" name="Task Name" dataDxfId="11"/>
+    <tableColumn id="3" name="BT 0.1" dataDxfId="10"/>
+    <tableColumn id="4" name="BT 0.2" dataDxfId="9"/>
+    <tableColumn id="5" name="BT 0.3" dataDxfId="8"/>
+    <tableColumn id="6" name="Break Down Notes" dataDxfId="7"/>
+    <tableColumn id="7" name="Completion Hours" dataDxfId="6"/>
+    <tableColumn id="8" name="Current Progress" dataDxfId="5"/>
+    <tableColumn id="9" name="Expected Completion Date" dataDxfId="4"/>
+    <tableColumn id="10" name="Real Completion Date" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2120,10 +2204,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:M253"/>
+  <dimension ref="A1:N253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="97" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="97" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,52 +2220,54 @@
     <col min="6" max="6" width="29.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="29.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="33.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" style="1" customWidth="1"/>
-    <col min="11" max="11" width="29.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="27.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="30.140625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="1"/>
+    <col min="9" max="9" width="48.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" style="1" customWidth="1"/>
+    <col min="12" max="12" width="29.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="27.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="30.140625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:13" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="3:13" s="3" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="3:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:14" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:14" s="3" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D4" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="11">
         <f ca="1">TODAY()</f>
-        <v>43257</v>
-      </c>
-      <c r="I4" s="1" t="s">
+        <v>43258</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="3:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="4">
-        <v>43198</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="I5" s="2"/>
+      <c r="J5" s="4">
+        <v>43290</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
@@ -2201,22 +2287,25 @@
         <v>9</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="3:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="12"/>
       <c r="D8" s="1" t="s">
         <v>12</v>
@@ -2224,387 +2313,387 @@
       <c r="H8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="80">
-        <f ca="1">ABS(_xlfn.DAYS(TODAY(), L8)*24)</f>
-        <v>504</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="80">
+        <f ca="1">ABS(_xlfn.DAYS(TODAY(), M8)*24)</f>
+        <v>528</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="8">
+      <c r="L8" s="8">
         <v>1</v>
       </c>
-      <c r="L8" s="20">
+      <c r="M8" s="20">
         <v>43236</v>
       </c>
-      <c r="M8" s="29">
+      <c r="N8" s="29">
         <v>43236</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C9" s="12"/>
       <c r="D9" s="5"/>
       <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="80"/>
-      <c r="K9" s="7">
+      <c r="J9" s="80"/>
+      <c r="L9" s="7">
         <v>1</v>
       </c>
-      <c r="L9" s="9"/>
       <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="12"/>
       <c r="D10" s="5"/>
       <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="80"/>
-      <c r="K10" s="7">
+      <c r="J10" s="80"/>
+      <c r="L10" s="7">
         <v>1</v>
       </c>
-      <c r="L10" s="9"/>
       <c r="M10" s="9"/>
-    </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="9"/>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C11" s="12"/>
       <c r="D11" s="5"/>
       <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="80"/>
-      <c r="K11" s="7">
+      <c r="J11" s="80"/>
+      <c r="L11" s="7">
         <v>1</v>
       </c>
-      <c r="L11" s="9"/>
       <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" s="12"/>
       <c r="D12" s="5"/>
       <c r="E12" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="I12" s="80"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="9"/>
+      <c r="J12" s="80"/>
+      <c r="L12" s="7"/>
       <c r="M12" s="9"/>
-    </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C13" s="14"/>
-      <c r="I13" s="80"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="9"/>
+      <c r="J13" s="80"/>
+      <c r="L13" s="7"/>
       <c r="M13" s="9"/>
-    </row>
-    <row r="14" spans="3:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="3:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="15"/>
       <c r="D14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="80">
-        <f ca="1">ABS(_xlfn.DAYS(TODAY(), L14)*24)</f>
-        <v>24</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="80">
+        <f ca="1">ABS(_xlfn.DAYS(TODAY(), M14)*24)</f>
+        <v>48</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="7">
+      <c r="L14" s="7">
         <v>0.2</v>
       </c>
-      <c r="L14" s="20">
+      <c r="M14" s="20">
         <v>43256</v>
       </c>
-      <c r="M14" s="28">
+      <c r="N14" s="28">
         <v>43256</v>
       </c>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C15" s="15"/>
       <c r="D15" s="5"/>
       <c r="E15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="80"/>
-      <c r="K15" s="7">
+      <c r="J15" s="80"/>
+      <c r="L15" s="7">
         <v>1</v>
       </c>
-      <c r="L15" s="9"/>
       <c r="M15" s="9"/>
-    </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C16" s="15"/>
       <c r="D16" s="5"/>
       <c r="E16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="80"/>
-      <c r="K16" s="7">
+      <c r="J16" s="80"/>
+      <c r="L16" s="7">
         <v>0</v>
       </c>
-      <c r="L16" s="9"/>
       <c r="M16" s="9"/>
-    </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17" s="15"/>
       <c r="D17" s="5"/>
       <c r="E17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="80"/>
-      <c r="K17" s="7">
+      <c r="J17" s="80"/>
+      <c r="L17" s="7">
         <v>0</v>
       </c>
-      <c r="L17" s="9"/>
       <c r="M17" s="9"/>
-    </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" s="15"/>
       <c r="D18" s="5"/>
       <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="80"/>
-      <c r="K18" s="7">
+      <c r="J18" s="80"/>
+      <c r="L18" s="7">
         <v>0.3</v>
       </c>
-      <c r="L18" s="9"/>
       <c r="M18" s="9"/>
-    </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C19" s="15"/>
       <c r="D19" s="5"/>
       <c r="E19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="80"/>
-      <c r="K19" s="7">
+      <c r="J19" s="80"/>
+      <c r="L19" s="7">
         <v>0.2</v>
       </c>
-      <c r="L19" s="9"/>
       <c r="M19" s="9"/>
-    </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C20" s="15"/>
       <c r="D20" s="5"/>
       <c r="E20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="80"/>
-      <c r="K20" s="7">
+      <c r="J20" s="80"/>
+      <c r="L20" s="7">
         <v>0</v>
       </c>
-      <c r="L20" s="9"/>
       <c r="M20" s="9"/>
-    </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I21" s="80"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="9"/>
+      <c r="N20" s="9"/>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J21" s="80"/>
+      <c r="L21" s="7"/>
       <c r="M21" s="9"/>
-    </row>
-    <row r="22" spans="3:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N21" s="9"/>
+    </row>
+    <row r="22" spans="3:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="13"/>
       <c r="D22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="80">
-        <f ca="1">ABS(_xlfn.DAYS(TODAY(), L22)*24)</f>
-        <v>336</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="80">
+        <f ca="1">ABS(_xlfn.DAYS(TODAY(), M22)*24)</f>
+        <v>360</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K22" s="7">
+      <c r="L22" s="7">
         <v>1</v>
       </c>
-      <c r="L22" s="20">
+      <c r="M22" s="20">
         <v>43243</v>
       </c>
-      <c r="M22" s="28">
+      <c r="N22" s="28">
         <v>43245</v>
       </c>
     </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C23" s="13"/>
       <c r="D23" s="5"/>
       <c r="E23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I23" s="80"/>
-      <c r="K23" s="7">
+      <c r="J23" s="80"/>
+      <c r="L23" s="7">
         <v>1</v>
       </c>
-      <c r="L23" s="9"/>
       <c r="M23" s="9"/>
-    </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="9"/>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C24" s="13"/>
       <c r="D24" s="5"/>
       <c r="E24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I24" s="80"/>
-      <c r="K24" s="7">
+      <c r="J24" s="80"/>
+      <c r="L24" s="7">
         <v>1</v>
       </c>
-      <c r="L24" s="9"/>
       <c r="M24" s="9"/>
-    </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="9"/>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C25" s="13"/>
       <c r="D25" s="5"/>
       <c r="E25" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="I25" s="80"/>
-      <c r="K25" s="7">
+      <c r="J25" s="80"/>
+      <c r="L25" s="7">
         <v>1</v>
       </c>
-      <c r="L25" s="9"/>
       <c r="M25" s="9"/>
-    </row>
-    <row r="26" spans="3:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N25" s="9"/>
+    </row>
+    <row r="26" spans="3:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C26" s="13"/>
       <c r="D26" s="5"/>
       <c r="E26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="80"/>
-      <c r="K26" s="7">
+      <c r="J26" s="80"/>
+      <c r="L26" s="7">
         <v>1</v>
       </c>
-      <c r="L26" s="9"/>
       <c r="M26" s="9"/>
-    </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="9"/>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C27" s="13"/>
       <c r="D27" s="5"/>
       <c r="E27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I27" s="80"/>
-      <c r="K27" s="7">
+      <c r="J27" s="80"/>
+      <c r="L27" s="7">
         <v>1</v>
       </c>
-      <c r="L27" s="9"/>
       <c r="M27" s="9"/>
-    </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="9"/>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C28" s="13"/>
       <c r="D28" s="5"/>
       <c r="E28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I28" s="80"/>
-      <c r="K28" s="7">
+      <c r="J28" s="80"/>
+      <c r="L28" s="7">
         <v>1</v>
       </c>
-      <c r="L28" s="9"/>
       <c r="M28" s="9"/>
-    </row>
-    <row r="29" spans="3:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N28" s="9"/>
+    </row>
+    <row r="29" spans="3:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C29" s="13"/>
       <c r="D29" s="5"/>
       <c r="E29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="80"/>
-      <c r="K29" s="7">
+      <c r="J29" s="80"/>
+      <c r="L29" s="7">
         <v>1</v>
       </c>
-      <c r="L29" s="9"/>
       <c r="M29" s="9"/>
-    </row>
-    <row r="30" spans="3:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N29" s="9"/>
+    </row>
+    <row r="30" spans="3:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C30" s="13"/>
       <c r="D30" s="5"/>
       <c r="E30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I30" s="80"/>
-      <c r="K30" s="7">
+      <c r="J30" s="80"/>
+      <c r="L30" s="7">
         <v>1</v>
       </c>
-      <c r="L30" s="9"/>
       <c r="M30" s="9"/>
-    </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N30" s="9"/>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C31" s="13"/>
       <c r="D31" s="5"/>
       <c r="E31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I31" s="80"/>
-      <c r="K31" s="7">
+      <c r="J31" s="80"/>
+      <c r="L31" s="7">
         <v>1</v>
       </c>
-      <c r="L31" s="9"/>
       <c r="M31" s="9"/>
-    </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I32" s="80"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="9"/>
+      <c r="N31" s="9"/>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J32" s="80"/>
+      <c r="L32" s="7"/>
       <c r="M32" s="9"/>
-    </row>
-    <row r="33" spans="3:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N32" s="9"/>
+    </row>
+    <row r="33" spans="3:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I33" s="80">
-        <f ca="1">ABS(_xlfn.DAYS(TODAY(), L33)*24)</f>
-        <v>96</v>
-      </c>
-      <c r="J33" s="1" t="s">
+      <c r="J33" s="80">
+        <f ca="1">ABS(_xlfn.DAYS(TODAY(), M33)*24)</f>
+        <v>72</v>
+      </c>
+      <c r="K33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K33" s="7">
+      <c r="L33" s="7">
         <v>0.1</v>
       </c>
-      <c r="L33" s="20">
+      <c r="M33" s="20">
         <v>43261</v>
       </c>
-      <c r="M33" s="9"/>
-    </row>
-    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="9"/>
+    </row>
+    <row r="34" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C34" s="13"/>
       <c r="D34" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I34" s="80"/>
-      <c r="K34" s="7">
+      <c r="J34" s="80"/>
+      <c r="L34" s="7">
         <v>0</v>
       </c>
-      <c r="L34" s="20"/>
-      <c r="M34" s="9"/>
-    </row>
-    <row r="35" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="M34" s="20"/>
+      <c r="N34" s="9"/>
+    </row>
+    <row r="35" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C35" s="13"/>
       <c r="E35" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I35" s="80"/>
-      <c r="K35" s="7">
+      <c r="J35" s="80"/>
+      <c r="L35" s="7">
         <v>0</v>
       </c>
-      <c r="L35" s="20"/>
-      <c r="M35" s="9"/>
-    </row>
-    <row r="36" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="M35" s="20"/>
+      <c r="N35" s="9"/>
+    </row>
+    <row r="36" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C36" s="13"/>
       <c r="D36" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I36" s="80"/>
-      <c r="K36" s="7">
+      <c r="J36" s="80"/>
+      <c r="L36" s="7">
         <v>1</v>
       </c>
-      <c r="L36" s="20"/>
-      <c r="M36" s="9"/>
-    </row>
-    <row r="37" spans="3:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M36" s="20"/>
+      <c r="N36" s="9"/>
+    </row>
+    <row r="37" spans="3:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="13"/>
       <c r="D37" s="5"/>
       <c r="E37" s="120" t="s">
@@ -2613,16 +2702,16 @@
       <c r="F37" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="I37" s="80"/>
-      <c r="K37" s="7">
+      <c r="J37" s="80"/>
+      <c r="L37" s="7">
         <v>1</v>
       </c>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9">
+      <c r="M37" s="9"/>
+      <c r="N37" s="9">
         <v>43254</v>
       </c>
     </row>
-    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C38" s="13"/>
       <c r="D38" s="5"/>
       <c r="E38" s="120" t="s">
@@ -2631,14 +2720,14 @@
       <c r="H38" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I38" s="80"/>
-      <c r="K38" s="7">
+      <c r="J38" s="80"/>
+      <c r="L38" s="7">
         <v>1</v>
       </c>
-      <c r="L38" s="9"/>
       <c r="M38" s="9"/>
-    </row>
-    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N38" s="9"/>
+    </row>
+    <row r="39" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C39" s="13"/>
       <c r="D39" s="5"/>
       <c r="E39" s="120" t="s">
@@ -2647,12 +2736,12 @@
       <c r="H39" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I39" s="80"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="9"/>
+      <c r="J39" s="80"/>
+      <c r="L39" s="7"/>
       <c r="M39" s="9"/>
-    </row>
-    <row r="40" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N39" s="9"/>
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C40" s="13"/>
       <c r="D40" s="5"/>
       <c r="E40" s="120" t="s">
@@ -2661,12 +2750,12 @@
       <c r="H40" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I40" s="80"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="9"/>
+      <c r="J40" s="80"/>
+      <c r="L40" s="7"/>
       <c r="M40" s="9"/>
-    </row>
-    <row r="41" spans="3:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N40" s="9"/>
+    </row>
+    <row r="41" spans="3:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="119"/>
       <c r="D41" s="5"/>
       <c r="E41" s="120" t="s">
@@ -2675,16 +2764,16 @@
       <c r="H41" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I41" s="80"/>
-      <c r="K41" s="7">
+      <c r="J41" s="80"/>
+      <c r="L41" s="7">
         <v>0.1</v>
       </c>
-      <c r="L41" s="9">
+      <c r="M41" s="9">
         <v>43256</v>
       </c>
-      <c r="M41" s="9"/>
-    </row>
-    <row r="42" spans="3:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N41" s="9"/>
+    </row>
+    <row r="42" spans="3:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="119"/>
       <c r="D42" s="5"/>
       <c r="E42" s="120" t="s">
@@ -2693,80 +2782,83 @@
       <c r="H42" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I42" s="80"/>
-      <c r="K42" s="7">
+      <c r="J42" s="80"/>
+      <c r="L42" s="7">
         <v>0.1</v>
       </c>
-      <c r="L42" s="9">
+      <c r="M42" s="9">
         <v>43257</v>
       </c>
-      <c r="M42" s="9"/>
-    </row>
-    <row r="43" spans="3:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N42" s="9"/>
+    </row>
+    <row r="43" spans="3:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="119"/>
       <c r="D43" s="5"/>
       <c r="E43" s="120" t="s">
         <v>115</v>
       </c>
-      <c r="I43" s="80"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="9"/>
+      <c r="J43" s="80"/>
+      <c r="L43" s="7"/>
       <c r="M43" s="9"/>
-    </row>
-    <row r="44" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N43" s="9"/>
+    </row>
+    <row r="44" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C44" s="13"/>
       <c r="D44" s="5"/>
       <c r="E44" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="I44" s="80"/>
-      <c r="K44" s="7">
+      <c r="J44" s="80"/>
+      <c r="L44" s="7">
         <v>1</v>
       </c>
-      <c r="L44" s="9"/>
       <c r="M44" s="9"/>
-    </row>
-    <row r="45" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N44" s="9"/>
+    </row>
+    <row r="45" spans="3:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E45" s="120"/>
-      <c r="I45" s="80"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="9"/>
+      <c r="J45" s="80"/>
+      <c r="L45" s="7"/>
       <c r="M45" s="9"/>
-    </row>
-    <row r="46" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N45" s="9"/>
+    </row>
+    <row r="46" spans="3:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E46" s="14"/>
-      <c r="I46" s="80"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="9"/>
+      <c r="J46" s="80"/>
+      <c r="L46" s="7"/>
       <c r="M46" s="9"/>
-    </row>
-    <row r="47" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N46" s="9"/>
+    </row>
+    <row r="47" spans="3:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="92"/>
       <c r="E47" s="14"/>
-      <c r="I47" s="80"/>
-      <c r="J47" s="1">
+      <c r="J47" s="80">
+        <f ca="1">ABS(_xlfn.DAYS(TODAY(), M47)*24)</f>
+        <v>120</v>
+      </c>
+      <c r="K47" s="1">
         <v>50</v>
       </c>
-      <c r="K47" s="7">
+      <c r="L47" s="7">
         <v>0.2</v>
       </c>
-      <c r="L47" s="9">
+      <c r="M47" s="9">
         <v>43263</v>
       </c>
-      <c r="M47" s="9"/>
-    </row>
-    <row r="48" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N47" s="9"/>
+    </row>
+    <row r="48" spans="3:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="92"/>
       <c r="D48" s="82" t="s">
         <v>121</v>
       </c>
       <c r="E48" s="14"/>
-      <c r="I48" s="80"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="9"/>
+      <c r="J48" s="80"/>
+      <c r="L48" s="7"/>
       <c r="M48" s="9"/>
-    </row>
-    <row r="49" spans="3:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N48" s="9"/>
+    </row>
+    <row r="49" spans="3:14" ht="45" x14ac:dyDescent="0.25">
       <c r="C49" s="92"/>
       <c r="D49" s="1" t="s">
         <v>172</v>
@@ -2775,14 +2867,22 @@
       <c r="H49" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I49" s="80"/>
-      <c r="K49" s="7">
+      <c r="I49" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J49" s="80">
+        <f t="shared" ref="J48:J55" ca="1" si="0">ABS(_xlfn.DAYS(TODAY(), M49)*24)</f>
+        <v>192</v>
+      </c>
+      <c r="L49" s="7">
         <v>0</v>
       </c>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
-    </row>
-    <row r="50" spans="3:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="M49" s="9">
+        <v>43266</v>
+      </c>
+      <c r="N49" s="9"/>
+    </row>
+    <row r="50" spans="3:14" ht="60" x14ac:dyDescent="0.25">
       <c r="C50" s="92"/>
       <c r="D50" s="1" t="s">
         <v>122</v>
@@ -2796,14 +2896,22 @@
       <c r="G50" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I50" s="80"/>
-      <c r="K50" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
-    </row>
-    <row r="51" spans="3:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="I50" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="J50" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="L50" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="M50" s="9">
+        <v>43263</v>
+      </c>
+      <c r="N50" s="9"/>
+    </row>
+    <row r="51" spans="3:14" ht="60" x14ac:dyDescent="0.25">
       <c r="C51" s="92"/>
       <c r="D51" s="1" t="s">
         <v>126</v>
@@ -2820,14 +2928,22 @@
       <c r="H51" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="I51" s="80"/>
-      <c r="K51" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="L51" s="9"/>
-      <c r="M51" s="9"/>
-    </row>
-    <row r="52" spans="3:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="I51" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="J51" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="L51" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="M51" s="9">
+        <v>43263</v>
+      </c>
+      <c r="N51" s="9"/>
+    </row>
+    <row r="52" spans="3:14" ht="60" x14ac:dyDescent="0.25">
       <c r="C52" s="92"/>
       <c r="D52" s="1" t="s">
         <v>130</v>
@@ -2841,14 +2957,22 @@
       <c r="G52" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I52" s="80"/>
-      <c r="K52" s="7">
+      <c r="I52" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J52" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="L52" s="7">
         <v>0</v>
       </c>
-      <c r="L52" s="9"/>
-      <c r="M52" s="9"/>
-    </row>
-    <row r="53" spans="3:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="M52" s="9">
+        <v>43263</v>
+      </c>
+      <c r="N52" s="9"/>
+    </row>
+    <row r="53" spans="3:14" ht="60" x14ac:dyDescent="0.25">
       <c r="C53" s="92"/>
       <c r="D53" s="1" t="s">
         <v>134</v>
@@ -2859,170 +2983,197 @@
       <c r="F53" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I53" s="80"/>
-      <c r="K53" s="7">
+      <c r="I53" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="J53" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="L53" s="7">
         <v>0</v>
       </c>
-      <c r="L53" s="9"/>
-      <c r="M53" s="9"/>
-    </row>
-    <row r="54" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M53" s="9">
+        <v>43263</v>
+      </c>
+      <c r="N53" s="9"/>
+    </row>
+    <row r="54" spans="3:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="92"/>
       <c r="E54" s="14"/>
-      <c r="I54" s="80"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
-    </row>
-    <row r="55" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J54" s="80"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="9">
+        <v>43263</v>
+      </c>
+      <c r="N54" s="9"/>
+    </row>
+    <row r="55" spans="3:14" ht="60" x14ac:dyDescent="0.25">
       <c r="C55" s="92"/>
+      <c r="D55" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="E55" s="14"/>
-      <c r="I55" s="80"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="9"/>
-      <c r="M55" s="9"/>
-    </row>
-    <row r="56" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I55" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J55" s="80">
+        <f t="shared" ca="1" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="L55" s="7"/>
+      <c r="M55" s="9">
+        <v>43263</v>
+      </c>
+      <c r="N55" s="9"/>
+    </row>
+    <row r="56" spans="3:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="92"/>
       <c r="E56" s="14"/>
-      <c r="I56" s="80"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="9"/>
+      <c r="J56" s="80"/>
+      <c r="L56" s="7"/>
       <c r="M56" s="9"/>
-    </row>
-    <row r="57" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N56" s="9"/>
+    </row>
+    <row r="57" spans="3:14" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E57" s="14"/>
-      <c r="I57" s="80"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="9"/>
+      <c r="H57" s="121" t="s">
+        <v>185</v>
+      </c>
+      <c r="I57" s="121" t="s">
+        <v>184</v>
+      </c>
+      <c r="J57" s="80"/>
+      <c r="L57" s="7"/>
       <c r="M57" s="9"/>
-    </row>
-    <row r="58" spans="3:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N57" s="9"/>
+    </row>
+    <row r="58" spans="3:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E58" s="14"/>
-      <c r="I58" s="80"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="9"/>
+      <c r="J58" s="80"/>
+      <c r="L58" s="7"/>
       <c r="M58" s="9"/>
-    </row>
-    <row r="59" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N58" s="9"/>
+    </row>
+    <row r="59" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C59" s="16"/>
       <c r="D59" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I59" s="80">
-        <f ca="1">ABS(_xlfn.DAYS(TODAY(), L59)*24)</f>
-        <v>1584</v>
-      </c>
-      <c r="J59" s="1" t="s">
+      <c r="J59" s="80">
+        <f ca="1">ABS(_xlfn.DAYS(TODAY(), M59)*24)</f>
+        <v>1608</v>
+      </c>
+      <c r="K59" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K59" s="7"/>
-      <c r="L59" s="20">
+      <c r="L59" s="7"/>
+      <c r="M59" s="20">
         <v>43191</v>
       </c>
-      <c r="M59" s="9"/>
-    </row>
-    <row r="60" spans="3:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N59" s="9"/>
+    </row>
+    <row r="60" spans="3:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="16"/>
       <c r="D60" s="5"/>
       <c r="E60" s="81" t="s">
         <v>120</v>
       </c>
-      <c r="I60" s="80"/>
-      <c r="K60" s="7">
+      <c r="J60" s="80"/>
+      <c r="L60" s="7">
         <v>1</v>
       </c>
-      <c r="L60" s="20"/>
-      <c r="M60" s="9"/>
-    </row>
-    <row r="61" spans="3:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="M60" s="20"/>
+      <c r="N60" s="9"/>
+    </row>
+    <row r="61" spans="3:14" ht="45" x14ac:dyDescent="0.25">
       <c r="C61" s="16"/>
       <c r="D61" s="5"/>
       <c r="E61" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I61" s="80"/>
-      <c r="K61" s="7"/>
-      <c r="L61" s="9"/>
+      <c r="J61" s="80"/>
+      <c r="L61" s="7"/>
       <c r="M61" s="9"/>
-    </row>
-    <row r="62" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N61" s="9"/>
+    </row>
+    <row r="62" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C62" s="16"/>
       <c r="D62" s="5"/>
       <c r="E62" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I62" s="80"/>
-      <c r="K62" s="7">
+      <c r="J62" s="80"/>
+      <c r="L62" s="7">
         <v>1</v>
       </c>
-      <c r="L62" s="9"/>
       <c r="M62" s="9"/>
-    </row>
-    <row r="63" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N62" s="9"/>
+    </row>
+    <row r="63" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C63" s="16"/>
       <c r="D63" s="5"/>
       <c r="E63" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I63" s="80"/>
-      <c r="K63" s="7">
+      <c r="J63" s="80"/>
+      <c r="L63" s="7">
         <v>0</v>
       </c>
-      <c r="L63" s="9"/>
       <c r="M63" s="9"/>
-    </row>
-    <row r="64" spans="3:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N63" s="9"/>
+    </row>
+    <row r="64" spans="3:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C64" s="16"/>
       <c r="D64" s="5"/>
       <c r="F64" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I64" s="80"/>
-      <c r="K64" s="7"/>
-      <c r="L64" s="9"/>
+      <c r="J64" s="80"/>
+      <c r="L64" s="7"/>
       <c r="M64" s="9"/>
-    </row>
-    <row r="65" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N64" s="9"/>
+    </row>
+    <row r="65" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C65" s="16"/>
       <c r="D65" s="5"/>
       <c r="G65" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I65" s="80"/>
-      <c r="K65" s="7"/>
-      <c r="L65" s="9"/>
+      <c r="J65" s="80"/>
+      <c r="L65" s="7"/>
       <c r="M65" s="9"/>
-    </row>
-    <row r="66" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N65" s="9"/>
+    </row>
+    <row r="66" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C66" s="16"/>
       <c r="D66" s="5"/>
       <c r="E66" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I66" s="80"/>
-      <c r="K66" s="7"/>
-      <c r="L66" s="9"/>
+      <c r="J66" s="80"/>
+      <c r="L66" s="7"/>
       <c r="M66" s="9"/>
-    </row>
-    <row r="67" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N66" s="9"/>
+    </row>
+    <row r="67" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C67" s="16"/>
       <c r="D67" s="5"/>
       <c r="E67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I67" s="80"/>
-      <c r="K67" s="7"/>
-      <c r="L67" s="9"/>
+      <c r="J67" s="80"/>
+      <c r="L67" s="7"/>
       <c r="M67" s="9"/>
-    </row>
-    <row r="68" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I68" s="80"/>
-      <c r="K68" s="7"/>
-      <c r="L68" s="9"/>
+      <c r="N67" s="9"/>
+    </row>
+    <row r="68" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J68" s="80"/>
+      <c r="L68" s="7"/>
       <c r="M68" s="9"/>
-    </row>
-    <row r="69" spans="3:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N68" s="9"/>
+    </row>
+    <row r="69" spans="3:14" ht="45" x14ac:dyDescent="0.25">
       <c r="C69" s="17"/>
       <c r="D69" s="1" t="s">
         <v>43</v>
@@ -3030,1207 +3181,1201 @@
       <c r="H69" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I69" s="80">
-        <f t="shared" ref="I69:I80" ca="1" si="0">_xlfn.DAYS(TODAY(), L69)*24</f>
-        <v>1488</v>
-      </c>
-      <c r="J69" s="1" t="s">
+      <c r="J69" s="80"/>
+      <c r="K69" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K69" s="7"/>
-      <c r="L69" s="20">
+      <c r="L69" s="7"/>
+      <c r="M69" s="20">
         <v>43195</v>
       </c>
-      <c r="M69" s="9"/>
-    </row>
-    <row r="70" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N69" s="9"/>
+    </row>
+    <row r="70" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C70" s="17"/>
       <c r="D70" s="26"/>
       <c r="E70" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I70" s="80"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="9"/>
+      <c r="J70" s="80"/>
+      <c r="L70" s="7"/>
       <c r="M70" s="9"/>
-    </row>
-    <row r="71" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N70" s="9"/>
+    </row>
+    <row r="71" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C71" s="17"/>
       <c r="D71" s="26"/>
       <c r="E71" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I71" s="80"/>
-      <c r="K71" s="7"/>
-      <c r="L71" s="9"/>
+      <c r="J71" s="80"/>
+      <c r="L71" s="7"/>
       <c r="M71" s="9"/>
-    </row>
-    <row r="72" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N71" s="9"/>
+    </row>
+    <row r="72" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C72" s="17"/>
       <c r="D72" s="26"/>
       <c r="E72" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I72" s="80"/>
-      <c r="K72" s="7"/>
-      <c r="L72" s="9"/>
+      <c r="J72" s="80"/>
+      <c r="L72" s="7"/>
       <c r="M72" s="9"/>
-    </row>
-    <row r="73" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N72" s="9"/>
+    </row>
+    <row r="73" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C73" s="17"/>
       <c r="D73" s="26"/>
       <c r="F73" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I73" s="80"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="9"/>
+      <c r="J73" s="80"/>
+      <c r="L73" s="7"/>
       <c r="M73" s="9"/>
-    </row>
-    <row r="74" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N73" s="9"/>
+    </row>
+    <row r="74" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C74" s="17"/>
       <c r="D74" s="26"/>
       <c r="F74" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I74" s="80"/>
-      <c r="K74" s="7"/>
-      <c r="L74" s="9"/>
+      <c r="J74" s="80"/>
+      <c r="L74" s="7"/>
       <c r="M74" s="9"/>
-    </row>
-    <row r="75" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N74" s="9"/>
+    </row>
+    <row r="75" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C75" s="17"/>
       <c r="D75" s="26"/>
       <c r="E75" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I75" s="80"/>
-      <c r="K75" s="7"/>
-      <c r="L75" s="9"/>
+      <c r="J75" s="80"/>
+      <c r="L75" s="7"/>
       <c r="M75" s="9"/>
-    </row>
-    <row r="76" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N75" s="9"/>
+    </row>
+    <row r="76" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C76" s="17"/>
       <c r="D76" s="26"/>
       <c r="E76" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I76" s="80"/>
-      <c r="K76" s="7"/>
-      <c r="L76" s="9"/>
+      <c r="J76" s="80"/>
+      <c r="L76" s="7"/>
       <c r="M76" s="9"/>
-    </row>
-    <row r="77" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N76" s="9"/>
+    </row>
+    <row r="77" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C77" s="17"/>
       <c r="D77" s="26"/>
       <c r="E77" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I77" s="80"/>
-      <c r="K77" s="7"/>
-      <c r="L77" s="9"/>
+      <c r="J77" s="80"/>
+      <c r="L77" s="7"/>
       <c r="M77" s="9"/>
-    </row>
-    <row r="78" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N77" s="9"/>
+    </row>
+    <row r="78" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C78" s="17"/>
       <c r="D78" s="26"/>
       <c r="E78" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I78" s="80"/>
-      <c r="K78" s="7"/>
-      <c r="L78" s="9"/>
+      <c r="J78" s="80"/>
+      <c r="L78" s="7"/>
       <c r="M78" s="9"/>
-    </row>
-    <row r="79" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I79" s="80"/>
-      <c r="K79" s="7"/>
-      <c r="L79" s="9"/>
+      <c r="N78" s="9"/>
+    </row>
+    <row r="79" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J79" s="80"/>
+      <c r="L79" s="7"/>
       <c r="M79" s="9"/>
-    </row>
-    <row r="80" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N79" s="9"/>
+    </row>
+    <row r="80" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C80" s="19"/>
       <c r="D80" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I80" s="80">
-        <f t="shared" ca="1" si="0"/>
-        <v>1416</v>
-      </c>
-      <c r="J80" s="1" t="s">
+      <c r="J80" s="80"/>
+      <c r="K80" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K80" s="7"/>
-      <c r="L80" s="20">
+      <c r="L80" s="7"/>
+      <c r="M80" s="20">
         <v>43198</v>
       </c>
-      <c r="M80" s="9"/>
-    </row>
-    <row r="81" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N80" s="9"/>
+    </row>
+    <row r="81" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C81" s="19"/>
       <c r="D81" s="5"/>
       <c r="E81" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I81" s="80"/>
-      <c r="K81" s="7"/>
-      <c r="L81" s="9"/>
+      <c r="J81" s="80"/>
+      <c r="L81" s="7"/>
       <c r="M81" s="9"/>
-    </row>
-    <row r="82" spans="3:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N81" s="9"/>
+    </row>
+    <row r="82" spans="3:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C82" s="19"/>
       <c r="D82" s="5"/>
       <c r="E82" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I82" s="80"/>
-      <c r="K82" s="7"/>
-      <c r="L82" s="9"/>
+      <c r="J82" s="80"/>
+      <c r="L82" s="7"/>
       <c r="M82" s="9"/>
-    </row>
-    <row r="83" spans="3:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N82" s="9"/>
+    </row>
+    <row r="83" spans="3:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C83" s="19"/>
       <c r="D83" s="5"/>
       <c r="E83" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I83" s="80"/>
-      <c r="K83" s="7"/>
-      <c r="L83" s="9"/>
+      <c r="J83" s="80"/>
+      <c r="L83" s="7"/>
       <c r="M83" s="9"/>
-    </row>
-    <row r="84" spans="3:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N83" s="9"/>
+    </row>
+    <row r="84" spans="3:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C84" s="19"/>
       <c r="D84" s="5"/>
       <c r="E84" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I84" s="80"/>
-      <c r="K84" s="7"/>
-      <c r="L84" s="9"/>
+      <c r="J84" s="80"/>
+      <c r="L84" s="7"/>
       <c r="M84" s="9"/>
-    </row>
-    <row r="85" spans="3:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N84" s="9"/>
+    </row>
+    <row r="85" spans="3:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C85" s="19"/>
       <c r="D85" s="5"/>
       <c r="E85" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I85" s="80"/>
-      <c r="K85" s="7"/>
-      <c r="L85" s="9"/>
+      <c r="J85" s="80"/>
+      <c r="L85" s="7"/>
       <c r="M85" s="9"/>
-    </row>
-    <row r="86" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I86" s="80"/>
-      <c r="K86" s="7"/>
-      <c r="L86" s="9"/>
+      <c r="N85" s="9"/>
+    </row>
+    <row r="86" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J86" s="80"/>
+      <c r="L86" s="7"/>
       <c r="M86" s="9"/>
-    </row>
-    <row r="87" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I87" s="80"/>
-      <c r="K87" s="7"/>
-      <c r="L87" s="9"/>
+      <c r="N86" s="9"/>
+    </row>
+    <row r="87" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J87" s="80"/>
+      <c r="L87" s="7"/>
       <c r="M87" s="9"/>
-    </row>
-    <row r="88" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I88" s="80"/>
-      <c r="K88" s="7"/>
-      <c r="L88" s="9"/>
+      <c r="N87" s="9"/>
+    </row>
+    <row r="88" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J88" s="80"/>
+      <c r="L88" s="7"/>
       <c r="M88" s="9"/>
-    </row>
-    <row r="89" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I89" s="80"/>
-      <c r="K89" s="7"/>
-      <c r="L89" s="9"/>
+      <c r="N88" s="9"/>
+    </row>
+    <row r="89" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J89" s="80"/>
+      <c r="L89" s="7"/>
       <c r="M89" s="9"/>
-    </row>
-    <row r="90" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I90" s="80"/>
-      <c r="K90" s="7"/>
-      <c r="L90" s="9"/>
+      <c r="N89" s="9"/>
+    </row>
+    <row r="90" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J90" s="80"/>
+      <c r="L90" s="7"/>
       <c r="M90" s="9"/>
-    </row>
-    <row r="91" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I91" s="80"/>
-      <c r="K91" s="7"/>
-      <c r="L91" s="9"/>
+      <c r="N90" s="9"/>
+    </row>
+    <row r="91" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J91" s="80"/>
+      <c r="L91" s="7"/>
       <c r="M91" s="9"/>
-    </row>
-    <row r="92" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I92" s="80"/>
-      <c r="K92" s="7"/>
-      <c r="L92" s="9"/>
+      <c r="N91" s="9"/>
+    </row>
+    <row r="92" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J92" s="80"/>
+      <c r="L92" s="7"/>
       <c r="M92" s="9"/>
-    </row>
-    <row r="93" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I93" s="80"/>
-      <c r="K93" s="7"/>
-      <c r="L93" s="9"/>
+      <c r="N92" s="9"/>
+    </row>
+    <row r="93" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J93" s="80"/>
+      <c r="L93" s="7"/>
       <c r="M93" s="9"/>
-    </row>
-    <row r="94" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I94" s="80"/>
-      <c r="K94" s="7"/>
-      <c r="L94" s="9"/>
+      <c r="N93" s="9"/>
+    </row>
+    <row r="94" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J94" s="80"/>
+      <c r="L94" s="7"/>
       <c r="M94" s="9"/>
-    </row>
-    <row r="95" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I95" s="80"/>
-      <c r="K95" s="7"/>
-      <c r="L95" s="9"/>
+      <c r="N94" s="9"/>
+    </row>
+    <row r="95" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J95" s="80"/>
+      <c r="L95" s="7"/>
       <c r="M95" s="9"/>
-    </row>
-    <row r="96" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I96" s="80"/>
-      <c r="K96" s="7"/>
-      <c r="L96" s="9"/>
+      <c r="N95" s="9"/>
+    </row>
+    <row r="96" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J96" s="80"/>
+      <c r="L96" s="7"/>
       <c r="M96" s="9"/>
-    </row>
-    <row r="97" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I97" s="80"/>
-      <c r="K97" s="7"/>
-      <c r="L97" s="9"/>
+      <c r="N96" s="9"/>
+    </row>
+    <row r="97" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J97" s="80"/>
+      <c r="L97" s="7"/>
       <c r="M97" s="9"/>
-    </row>
-    <row r="98" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I98" s="80"/>
-      <c r="K98" s="7"/>
-      <c r="L98" s="9"/>
+      <c r="N97" s="9"/>
+    </row>
+    <row r="98" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J98" s="80"/>
+      <c r="L98" s="7"/>
       <c r="M98" s="9"/>
-    </row>
-    <row r="99" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I99" s="80"/>
-      <c r="K99" s="7"/>
-      <c r="L99" s="9"/>
+      <c r="N98" s="9"/>
+    </row>
+    <row r="99" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J99" s="80"/>
+      <c r="L99" s="7"/>
       <c r="M99" s="9"/>
-    </row>
-    <row r="100" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I100" s="80"/>
-      <c r="K100" s="7"/>
-      <c r="L100" s="9"/>
+      <c r="N99" s="9"/>
+    </row>
+    <row r="100" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J100" s="80"/>
+      <c r="L100" s="7"/>
       <c r="M100" s="9"/>
-    </row>
-    <row r="101" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I101" s="80"/>
-      <c r="K101" s="7"/>
-      <c r="L101" s="9"/>
+      <c r="N100" s="9"/>
+    </row>
+    <row r="101" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J101" s="80"/>
+      <c r="L101" s="7"/>
       <c r="M101" s="9"/>
-    </row>
-    <row r="102" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I102" s="80"/>
-      <c r="K102" s="7"/>
-      <c r="L102" s="9"/>
+      <c r="N101" s="9"/>
+    </row>
+    <row r="102" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J102" s="80"/>
+      <c r="L102" s="7"/>
       <c r="M102" s="9"/>
-    </row>
-    <row r="103" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I103" s="80"/>
-      <c r="K103" s="7"/>
-      <c r="L103" s="9"/>
+      <c r="N102" s="9"/>
+    </row>
+    <row r="103" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J103" s="80"/>
+      <c r="L103" s="7"/>
       <c r="M103" s="9"/>
-    </row>
-    <row r="104" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I104" s="80"/>
-      <c r="K104" s="7"/>
-      <c r="L104" s="9"/>
+      <c r="N103" s="9"/>
+    </row>
+    <row r="104" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J104" s="80"/>
+      <c r="L104" s="7"/>
       <c r="M104" s="9"/>
-    </row>
-    <row r="105" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I105" s="80"/>
-      <c r="K105" s="7"/>
-      <c r="L105" s="9"/>
+      <c r="N104" s="9"/>
+    </row>
+    <row r="105" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J105" s="80"/>
+      <c r="L105" s="7"/>
       <c r="M105" s="9"/>
-    </row>
-    <row r="106" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I106" s="80"/>
-      <c r="K106" s="7"/>
-      <c r="L106" s="9"/>
+      <c r="N105" s="9"/>
+    </row>
+    <row r="106" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J106" s="80"/>
+      <c r="L106" s="7"/>
       <c r="M106" s="9"/>
-    </row>
-    <row r="107" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I107" s="80"/>
-      <c r="K107" s="7"/>
-      <c r="L107" s="9"/>
+      <c r="N106" s="9"/>
+    </row>
+    <row r="107" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J107" s="80"/>
+      <c r="L107" s="7"/>
       <c r="M107" s="9"/>
-    </row>
-    <row r="108" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I108" s="80"/>
-      <c r="K108" s="7"/>
-      <c r="L108" s="9"/>
+      <c r="N107" s="9"/>
+    </row>
+    <row r="108" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J108" s="80"/>
+      <c r="L108" s="7"/>
       <c r="M108" s="9"/>
-    </row>
-    <row r="109" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I109" s="80"/>
-      <c r="K109" s="7"/>
-      <c r="L109" s="9"/>
+      <c r="N108" s="9"/>
+    </row>
+    <row r="109" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J109" s="80"/>
+      <c r="L109" s="7"/>
       <c r="M109" s="9"/>
-    </row>
-    <row r="110" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I110" s="80"/>
-      <c r="K110" s="7"/>
-      <c r="L110" s="9"/>
+      <c r="N109" s="9"/>
+    </row>
+    <row r="110" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J110" s="80"/>
+      <c r="L110" s="7"/>
       <c r="M110" s="9"/>
-    </row>
-    <row r="111" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I111" s="80"/>
-      <c r="K111" s="7"/>
-      <c r="L111" s="9"/>
+      <c r="N110" s="9"/>
+    </row>
+    <row r="111" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J111" s="80"/>
+      <c r="L111" s="7"/>
       <c r="M111" s="9"/>
-    </row>
-    <row r="112" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I112" s="80"/>
-      <c r="K112" s="7"/>
-      <c r="L112" s="9"/>
+      <c r="N111" s="9"/>
+    </row>
+    <row r="112" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J112" s="80"/>
+      <c r="L112" s="7"/>
       <c r="M112" s="9"/>
-    </row>
-    <row r="113" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I113" s="80"/>
-      <c r="K113" s="7"/>
-      <c r="L113" s="9"/>
+      <c r="N112" s="9"/>
+    </row>
+    <row r="113" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J113" s="80"/>
+      <c r="L113" s="7"/>
       <c r="M113" s="9"/>
-    </row>
-    <row r="114" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I114" s="80"/>
-      <c r="K114" s="7"/>
-      <c r="L114" s="9"/>
+      <c r="N113" s="9"/>
+    </row>
+    <row r="114" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J114" s="80"/>
+      <c r="L114" s="7"/>
       <c r="M114" s="9"/>
-    </row>
-    <row r="115" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I115" s="80"/>
-      <c r="K115" s="7"/>
-      <c r="L115" s="9"/>
+      <c r="N114" s="9"/>
+    </row>
+    <row r="115" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J115" s="80"/>
+      <c r="L115" s="7"/>
       <c r="M115" s="9"/>
-    </row>
-    <row r="116" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I116" s="80"/>
-      <c r="K116" s="7"/>
-      <c r="L116" s="9"/>
+      <c r="N115" s="9"/>
+    </row>
+    <row r="116" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J116" s="80"/>
+      <c r="L116" s="7"/>
       <c r="M116" s="9"/>
-    </row>
-    <row r="117" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I117" s="80"/>
-      <c r="K117" s="7"/>
-      <c r="L117" s="9"/>
+      <c r="N116" s="9"/>
+    </row>
+    <row r="117" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J117" s="80"/>
+      <c r="L117" s="7"/>
       <c r="M117" s="9"/>
-    </row>
-    <row r="118" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I118" s="80"/>
-      <c r="K118" s="7"/>
-      <c r="L118" s="9"/>
+      <c r="N117" s="9"/>
+    </row>
+    <row r="118" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J118" s="80"/>
+      <c r="L118" s="7"/>
       <c r="M118" s="9"/>
-    </row>
-    <row r="119" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I119" s="80"/>
-      <c r="K119" s="7"/>
-      <c r="L119" s="9"/>
+      <c r="N118" s="9"/>
+    </row>
+    <row r="119" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J119" s="80"/>
+      <c r="L119" s="7"/>
       <c r="M119" s="9"/>
-    </row>
-    <row r="120" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I120" s="80"/>
-      <c r="K120" s="7"/>
-      <c r="L120" s="9"/>
+      <c r="N119" s="9"/>
+    </row>
+    <row r="120" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J120" s="80"/>
+      <c r="L120" s="7"/>
       <c r="M120" s="9"/>
-    </row>
-    <row r="121" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I121" s="80"/>
-      <c r="K121" s="7"/>
-      <c r="L121" s="9"/>
+      <c r="N120" s="9"/>
+    </row>
+    <row r="121" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J121" s="80"/>
+      <c r="L121" s="7"/>
       <c r="M121" s="9"/>
-    </row>
-    <row r="122" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I122" s="80"/>
-      <c r="K122" s="7"/>
-      <c r="L122" s="9"/>
+      <c r="N121" s="9"/>
+    </row>
+    <row r="122" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J122" s="80"/>
+      <c r="L122" s="7"/>
       <c r="M122" s="9"/>
-    </row>
-    <row r="123" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I123" s="80"/>
-      <c r="K123" s="7"/>
-      <c r="L123" s="9"/>
+      <c r="N122" s="9"/>
+    </row>
+    <row r="123" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J123" s="80"/>
+      <c r="L123" s="7"/>
       <c r="M123" s="9"/>
-    </row>
-    <row r="124" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I124" s="80"/>
-      <c r="K124" s="7"/>
-      <c r="L124" s="9"/>
+      <c r="N123" s="9"/>
+    </row>
+    <row r="124" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J124" s="80"/>
+      <c r="L124" s="7"/>
       <c r="M124" s="9"/>
-    </row>
-    <row r="125" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I125" s="80"/>
-      <c r="K125" s="7"/>
-      <c r="L125" s="9"/>
+      <c r="N124" s="9"/>
+    </row>
+    <row r="125" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J125" s="80"/>
+      <c r="L125" s="7"/>
       <c r="M125" s="9"/>
-    </row>
-    <row r="126" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I126" s="80"/>
-      <c r="K126" s="7"/>
-      <c r="L126" s="9"/>
+      <c r="N125" s="9"/>
+    </row>
+    <row r="126" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J126" s="80"/>
+      <c r="L126" s="7"/>
       <c r="M126" s="9"/>
-    </row>
-    <row r="127" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I127" s="80"/>
-      <c r="K127" s="7"/>
-      <c r="L127" s="9"/>
+      <c r="N126" s="9"/>
+    </row>
+    <row r="127" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J127" s="80"/>
+      <c r="L127" s="7"/>
       <c r="M127" s="9"/>
-    </row>
-    <row r="128" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I128" s="80"/>
-      <c r="K128" s="7"/>
-      <c r="L128" s="9"/>
+      <c r="N127" s="9"/>
+    </row>
+    <row r="128" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J128" s="80"/>
+      <c r="L128" s="7"/>
       <c r="M128" s="9"/>
-    </row>
-    <row r="129" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I129" s="80"/>
-      <c r="K129" s="7"/>
-      <c r="L129" s="9"/>
+      <c r="N128" s="9"/>
+    </row>
+    <row r="129" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J129" s="80"/>
+      <c r="L129" s="7"/>
       <c r="M129" s="9"/>
-    </row>
-    <row r="130" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I130" s="80"/>
-      <c r="K130" s="7"/>
-      <c r="L130" s="9"/>
+      <c r="N129" s="9"/>
+    </row>
+    <row r="130" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J130" s="80"/>
+      <c r="L130" s="7"/>
       <c r="M130" s="9"/>
-    </row>
-    <row r="131" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I131" s="80"/>
-      <c r="K131" s="7"/>
-      <c r="L131" s="9"/>
+      <c r="N130" s="9"/>
+    </row>
+    <row r="131" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J131" s="80"/>
+      <c r="L131" s="7"/>
       <c r="M131" s="9"/>
-    </row>
-    <row r="132" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I132" s="80"/>
-      <c r="K132" s="7"/>
-      <c r="L132" s="9"/>
+      <c r="N131" s="9"/>
+    </row>
+    <row r="132" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J132" s="80"/>
+      <c r="L132" s="7"/>
       <c r="M132" s="9"/>
-    </row>
-    <row r="133" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I133" s="80"/>
-      <c r="K133" s="7"/>
-      <c r="L133" s="9"/>
+      <c r="N132" s="9"/>
+    </row>
+    <row r="133" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J133" s="80"/>
+      <c r="L133" s="7"/>
       <c r="M133" s="9"/>
-    </row>
-    <row r="134" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I134" s="80"/>
-      <c r="K134" s="7"/>
-      <c r="L134" s="9"/>
+      <c r="N133" s="9"/>
+    </row>
+    <row r="134" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J134" s="80"/>
+      <c r="L134" s="7"/>
       <c r="M134" s="9"/>
-    </row>
-    <row r="135" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I135" s="80"/>
-      <c r="K135" s="7"/>
-      <c r="L135" s="9"/>
+      <c r="N134" s="9"/>
+    </row>
+    <row r="135" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J135" s="80"/>
+      <c r="L135" s="7"/>
       <c r="M135" s="9"/>
-    </row>
-    <row r="136" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I136" s="80"/>
-      <c r="K136" s="7"/>
-      <c r="L136" s="9"/>
+      <c r="N135" s="9"/>
+    </row>
+    <row r="136" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J136" s="80"/>
+      <c r="L136" s="7"/>
       <c r="M136" s="9"/>
-    </row>
-    <row r="137" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I137" s="80"/>
-      <c r="K137" s="7"/>
-      <c r="L137" s="9"/>
+      <c r="N136" s="9"/>
+    </row>
+    <row r="137" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J137" s="80"/>
+      <c r="L137" s="7"/>
       <c r="M137" s="9"/>
-    </row>
-    <row r="138" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I138" s="80"/>
-      <c r="K138" s="7"/>
-      <c r="L138" s="9"/>
+      <c r="N137" s="9"/>
+    </row>
+    <row r="138" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J138" s="80"/>
+      <c r="L138" s="7"/>
       <c r="M138" s="9"/>
-    </row>
-    <row r="139" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I139" s="80"/>
-      <c r="K139" s="7"/>
-      <c r="L139" s="9"/>
+      <c r="N138" s="9"/>
+    </row>
+    <row r="139" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J139" s="80"/>
+      <c r="L139" s="7"/>
       <c r="M139" s="9"/>
-    </row>
-    <row r="140" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I140" s="80"/>
-      <c r="K140" s="7"/>
-      <c r="L140" s="9"/>
+      <c r="N139" s="9"/>
+    </row>
+    <row r="140" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J140" s="80"/>
+      <c r="L140" s="7"/>
       <c r="M140" s="9"/>
-    </row>
-    <row r="141" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I141" s="80"/>
-      <c r="K141" s="7"/>
-      <c r="L141" s="9"/>
+      <c r="N140" s="9"/>
+    </row>
+    <row r="141" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J141" s="80"/>
+      <c r="L141" s="7"/>
       <c r="M141" s="9"/>
-    </row>
-    <row r="142" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I142" s="80"/>
-      <c r="K142" s="7"/>
-      <c r="L142" s="9"/>
+      <c r="N141" s="9"/>
+    </row>
+    <row r="142" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J142" s="80"/>
+      <c r="L142" s="7"/>
       <c r="M142" s="9"/>
-    </row>
-    <row r="143" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I143" s="80"/>
-      <c r="K143" s="7"/>
-      <c r="L143" s="9"/>
+      <c r="N142" s="9"/>
+    </row>
+    <row r="143" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J143" s="80"/>
+      <c r="L143" s="7"/>
       <c r="M143" s="9"/>
-    </row>
-    <row r="144" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I144" s="80"/>
-      <c r="K144" s="7"/>
-      <c r="L144" s="9"/>
+      <c r="N143" s="9"/>
+    </row>
+    <row r="144" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J144" s="80"/>
+      <c r="L144" s="7"/>
       <c r="M144" s="9"/>
-    </row>
-    <row r="145" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I145" s="80"/>
-      <c r="K145" s="7"/>
-      <c r="L145" s="9"/>
+      <c r="N144" s="9"/>
+    </row>
+    <row r="145" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J145" s="80"/>
+      <c r="L145" s="7"/>
       <c r="M145" s="9"/>
-    </row>
-    <row r="146" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I146" s="80"/>
-      <c r="K146" s="7"/>
-      <c r="L146" s="9"/>
+      <c r="N145" s="9"/>
+    </row>
+    <row r="146" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J146" s="80"/>
+      <c r="L146" s="7"/>
       <c r="M146" s="9"/>
-    </row>
-    <row r="147" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I147" s="80"/>
-      <c r="K147" s="7"/>
-      <c r="L147" s="9"/>
+      <c r="N146" s="9"/>
+    </row>
+    <row r="147" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J147" s="80"/>
+      <c r="L147" s="7"/>
       <c r="M147" s="9"/>
-    </row>
-    <row r="148" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I148" s="80"/>
-      <c r="K148" s="7"/>
-      <c r="L148" s="9"/>
+      <c r="N147" s="9"/>
+    </row>
+    <row r="148" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J148" s="80"/>
+      <c r="L148" s="7"/>
       <c r="M148" s="9"/>
-    </row>
-    <row r="149" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I149" s="80"/>
-      <c r="K149" s="7"/>
-      <c r="L149" s="9"/>
+      <c r="N148" s="9"/>
+    </row>
+    <row r="149" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J149" s="80"/>
+      <c r="L149" s="7"/>
       <c r="M149" s="9"/>
-    </row>
-    <row r="150" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I150" s="80"/>
-      <c r="K150" s="7"/>
-      <c r="L150" s="9"/>
+      <c r="N149" s="9"/>
+    </row>
+    <row r="150" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J150" s="80"/>
+      <c r="L150" s="7"/>
       <c r="M150" s="9"/>
-    </row>
-    <row r="151" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I151" s="80"/>
-      <c r="K151" s="7"/>
-      <c r="L151" s="9"/>
+      <c r="N150" s="9"/>
+    </row>
+    <row r="151" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J151" s="80"/>
+      <c r="L151" s="7"/>
       <c r="M151" s="9"/>
-    </row>
-    <row r="152" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I152" s="80"/>
-      <c r="K152" s="7"/>
-      <c r="L152" s="9"/>
+      <c r="N151" s="9"/>
+    </row>
+    <row r="152" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J152" s="80"/>
+      <c r="L152" s="7"/>
       <c r="M152" s="9"/>
-    </row>
-    <row r="153" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I153" s="80"/>
-      <c r="K153" s="7"/>
-      <c r="L153" s="9"/>
+      <c r="N152" s="9"/>
+    </row>
+    <row r="153" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J153" s="80"/>
+      <c r="L153" s="7"/>
       <c r="M153" s="9"/>
-    </row>
-    <row r="154" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I154" s="80"/>
-      <c r="K154" s="7"/>
-      <c r="L154" s="9"/>
+      <c r="N153" s="9"/>
+    </row>
+    <row r="154" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J154" s="80"/>
+      <c r="L154" s="7"/>
       <c r="M154" s="9"/>
-    </row>
-    <row r="155" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I155" s="80"/>
-      <c r="K155" s="7"/>
-      <c r="L155" s="9"/>
+      <c r="N154" s="9"/>
+    </row>
+    <row r="155" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J155" s="80"/>
+      <c r="L155" s="7"/>
       <c r="M155" s="9"/>
-    </row>
-    <row r="156" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I156" s="80"/>
-      <c r="K156" s="7"/>
-      <c r="L156" s="9"/>
+      <c r="N155" s="9"/>
+    </row>
+    <row r="156" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J156" s="80"/>
+      <c r="L156" s="7"/>
       <c r="M156" s="9"/>
-    </row>
-    <row r="157" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I157" s="80"/>
-      <c r="K157" s="7"/>
-      <c r="L157" s="9"/>
+      <c r="N156" s="9"/>
+    </row>
+    <row r="157" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J157" s="80"/>
+      <c r="L157" s="7"/>
       <c r="M157" s="9"/>
-    </row>
-    <row r="158" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I158" s="80"/>
-      <c r="K158" s="7"/>
-      <c r="L158" s="9"/>
+      <c r="N157" s="9"/>
+    </row>
+    <row r="158" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J158" s="80"/>
+      <c r="L158" s="7"/>
       <c r="M158" s="9"/>
-    </row>
-    <row r="159" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I159" s="80"/>
-      <c r="K159" s="7"/>
-      <c r="L159" s="9"/>
+      <c r="N158" s="9"/>
+    </row>
+    <row r="159" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J159" s="80"/>
+      <c r="L159" s="7"/>
       <c r="M159" s="9"/>
-    </row>
-    <row r="160" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I160" s="80"/>
-      <c r="K160" s="7"/>
-      <c r="L160" s="9"/>
+      <c r="N159" s="9"/>
+    </row>
+    <row r="160" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J160" s="80"/>
+      <c r="L160" s="7"/>
       <c r="M160" s="9"/>
-    </row>
-    <row r="161" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I161" s="80"/>
-      <c r="K161" s="7"/>
-      <c r="L161" s="9"/>
+      <c r="N160" s="9"/>
+    </row>
+    <row r="161" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J161" s="80"/>
+      <c r="L161" s="7"/>
       <c r="M161" s="9"/>
-    </row>
-    <row r="162" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I162" s="80"/>
-      <c r="K162" s="7"/>
-      <c r="L162" s="9"/>
+      <c r="N161" s="9"/>
+    </row>
+    <row r="162" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J162" s="80"/>
+      <c r="L162" s="7"/>
       <c r="M162" s="9"/>
-    </row>
-    <row r="163" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I163" s="80"/>
-      <c r="K163" s="7"/>
-      <c r="L163" s="9"/>
+      <c r="N162" s="9"/>
+    </row>
+    <row r="163" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J163" s="80"/>
+      <c r="L163" s="7"/>
       <c r="M163" s="9"/>
-    </row>
-    <row r="164" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I164" s="80"/>
-      <c r="K164" s="7"/>
-      <c r="L164" s="9"/>
+      <c r="N163" s="9"/>
+    </row>
+    <row r="164" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J164" s="80"/>
+      <c r="L164" s="7"/>
       <c r="M164" s="9"/>
-    </row>
-    <row r="165" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I165" s="80"/>
-      <c r="K165" s="7"/>
-      <c r="L165" s="9"/>
+      <c r="N164" s="9"/>
+    </row>
+    <row r="165" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J165" s="80"/>
+      <c r="L165" s="7"/>
       <c r="M165" s="9"/>
-    </row>
-    <row r="166" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I166" s="80"/>
-      <c r="K166" s="7"/>
-      <c r="L166" s="9"/>
+      <c r="N165" s="9"/>
+    </row>
+    <row r="166" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J166" s="80"/>
+      <c r="L166" s="7"/>
       <c r="M166" s="9"/>
-    </row>
-    <row r="167" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I167" s="80"/>
-      <c r="K167" s="7"/>
-      <c r="L167" s="9"/>
+      <c r="N166" s="9"/>
+    </row>
+    <row r="167" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J167" s="80"/>
+      <c r="L167" s="7"/>
       <c r="M167" s="9"/>
-    </row>
-    <row r="168" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I168" s="80"/>
-      <c r="K168" s="7"/>
-      <c r="L168" s="9"/>
+      <c r="N167" s="9"/>
+    </row>
+    <row r="168" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J168" s="80"/>
+      <c r="L168" s="7"/>
       <c r="M168" s="9"/>
-    </row>
-    <row r="169" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I169" s="80"/>
-      <c r="K169" s="7"/>
-      <c r="L169" s="9"/>
+      <c r="N168" s="9"/>
+    </row>
+    <row r="169" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J169" s="80"/>
+      <c r="L169" s="7"/>
       <c r="M169" s="9"/>
-    </row>
-    <row r="170" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I170" s="80"/>
-      <c r="K170" s="7"/>
-      <c r="L170" s="9"/>
+      <c r="N169" s="9"/>
+    </row>
+    <row r="170" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J170" s="80"/>
+      <c r="L170" s="7"/>
       <c r="M170" s="9"/>
-    </row>
-    <row r="171" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I171" s="80"/>
-      <c r="K171" s="7"/>
-      <c r="L171" s="9"/>
+      <c r="N170" s="9"/>
+    </row>
+    <row r="171" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J171" s="80"/>
+      <c r="L171" s="7"/>
       <c r="M171" s="9"/>
-    </row>
-    <row r="172" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I172" s="80"/>
-      <c r="K172" s="7"/>
-      <c r="L172" s="9"/>
+      <c r="N171" s="9"/>
+    </row>
+    <row r="172" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J172" s="80"/>
+      <c r="L172" s="7"/>
       <c r="M172" s="9"/>
-    </row>
-    <row r="173" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I173" s="80"/>
-      <c r="K173" s="7"/>
-      <c r="L173" s="9"/>
+      <c r="N172" s="9"/>
+    </row>
+    <row r="173" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J173" s="80"/>
+      <c r="L173" s="7"/>
       <c r="M173" s="9"/>
-    </row>
-    <row r="174" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I174" s="80"/>
-      <c r="K174" s="7"/>
-      <c r="L174" s="9"/>
+      <c r="N173" s="9"/>
+    </row>
+    <row r="174" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J174" s="80"/>
+      <c r="L174" s="7"/>
       <c r="M174" s="9"/>
-    </row>
-    <row r="175" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I175" s="80"/>
-      <c r="K175" s="7"/>
-      <c r="L175" s="9"/>
+      <c r="N174" s="9"/>
+    </row>
+    <row r="175" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J175" s="80"/>
+      <c r="L175" s="7"/>
       <c r="M175" s="9"/>
-    </row>
-    <row r="176" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I176" s="80"/>
-      <c r="K176" s="7"/>
-      <c r="L176" s="9"/>
+      <c r="N175" s="9"/>
+    </row>
+    <row r="176" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J176" s="80"/>
+      <c r="L176" s="7"/>
       <c r="M176" s="9"/>
-    </row>
-    <row r="177" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I177" s="80"/>
-      <c r="K177" s="7"/>
-      <c r="L177" s="9"/>
+      <c r="N176" s="9"/>
+    </row>
+    <row r="177" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J177" s="80"/>
+      <c r="L177" s="7"/>
       <c r="M177" s="9"/>
-    </row>
-    <row r="178" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I178" s="80"/>
-      <c r="K178" s="7"/>
-      <c r="L178" s="9"/>
+      <c r="N177" s="9"/>
+    </row>
+    <row r="178" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J178" s="80"/>
+      <c r="L178" s="7"/>
       <c r="M178" s="9"/>
-    </row>
-    <row r="179" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I179" s="80"/>
-      <c r="K179" s="7"/>
-      <c r="L179" s="9"/>
+      <c r="N178" s="9"/>
+    </row>
+    <row r="179" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J179" s="80"/>
+      <c r="L179" s="7"/>
       <c r="M179" s="9"/>
-    </row>
-    <row r="180" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I180" s="80"/>
-      <c r="K180" s="7"/>
-      <c r="L180" s="9"/>
+      <c r="N179" s="9"/>
+    </row>
+    <row r="180" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J180" s="80"/>
+      <c r="L180" s="7"/>
       <c r="M180" s="9"/>
-    </row>
-    <row r="181" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I181" s="80"/>
-      <c r="K181" s="7"/>
-      <c r="L181" s="9"/>
+      <c r="N180" s="9"/>
+    </row>
+    <row r="181" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J181" s="80"/>
+      <c r="L181" s="7"/>
       <c r="M181" s="9"/>
-    </row>
-    <row r="182" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I182" s="80"/>
-      <c r="K182" s="7"/>
-      <c r="L182" s="9"/>
+      <c r="N181" s="9"/>
+    </row>
+    <row r="182" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J182" s="80"/>
+      <c r="L182" s="7"/>
       <c r="M182" s="9"/>
-    </row>
-    <row r="183" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I183" s="80"/>
-      <c r="K183" s="7"/>
-      <c r="L183" s="9"/>
+      <c r="N182" s="9"/>
+    </row>
+    <row r="183" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J183" s="80"/>
+      <c r="L183" s="7"/>
       <c r="M183" s="9"/>
-    </row>
-    <row r="184" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I184" s="80"/>
-      <c r="K184" s="7"/>
-      <c r="L184" s="9"/>
+      <c r="N183" s="9"/>
+    </row>
+    <row r="184" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J184" s="80"/>
+      <c r="L184" s="7"/>
       <c r="M184" s="9"/>
-    </row>
-    <row r="185" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I185" s="80"/>
-      <c r="K185" s="7"/>
-      <c r="L185" s="9"/>
+      <c r="N184" s="9"/>
+    </row>
+    <row r="185" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J185" s="80"/>
+      <c r="L185" s="7"/>
       <c r="M185" s="9"/>
-    </row>
-    <row r="186" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I186" s="80"/>
-      <c r="K186" s="7"/>
-      <c r="L186" s="9"/>
+      <c r="N185" s="9"/>
+    </row>
+    <row r="186" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J186" s="80"/>
+      <c r="L186" s="7"/>
       <c r="M186" s="9"/>
-    </row>
-    <row r="187" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I187" s="80"/>
-      <c r="K187" s="7"/>
-      <c r="L187" s="9"/>
+      <c r="N186" s="9"/>
+    </row>
+    <row r="187" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J187" s="80"/>
+      <c r="L187" s="7"/>
       <c r="M187" s="9"/>
-    </row>
-    <row r="188" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I188" s="80"/>
-      <c r="K188" s="7"/>
-      <c r="L188" s="9"/>
+      <c r="N187" s="9"/>
+    </row>
+    <row r="188" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J188" s="80"/>
+      <c r="L188" s="7"/>
       <c r="M188" s="9"/>
-    </row>
-    <row r="189" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I189" s="80"/>
-      <c r="K189" s="7"/>
-      <c r="L189" s="9"/>
+      <c r="N188" s="9"/>
+    </row>
+    <row r="189" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J189" s="80"/>
+      <c r="L189" s="7"/>
       <c r="M189" s="9"/>
-    </row>
-    <row r="190" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I190" s="80"/>
-      <c r="K190" s="7"/>
-      <c r="L190" s="9"/>
+      <c r="N189" s="9"/>
+    </row>
+    <row r="190" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J190" s="80"/>
+      <c r="L190" s="7"/>
       <c r="M190" s="9"/>
-    </row>
-    <row r="191" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I191" s="80"/>
-      <c r="K191" s="7"/>
-      <c r="L191" s="9"/>
+      <c r="N190" s="9"/>
+    </row>
+    <row r="191" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J191" s="80"/>
+      <c r="L191" s="7"/>
       <c r="M191" s="9"/>
-    </row>
-    <row r="192" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I192" s="80"/>
-      <c r="K192" s="7"/>
-      <c r="L192" s="9"/>
+      <c r="N191" s="9"/>
+    </row>
+    <row r="192" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J192" s="80"/>
+      <c r="L192" s="7"/>
       <c r="M192" s="9"/>
-    </row>
-    <row r="193" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I193" s="80"/>
-      <c r="K193" s="7"/>
-      <c r="L193" s="9"/>
+      <c r="N192" s="9"/>
+    </row>
+    <row r="193" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J193" s="80"/>
+      <c r="L193" s="7"/>
       <c r="M193" s="9"/>
-    </row>
-    <row r="194" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I194" s="80"/>
-      <c r="K194" s="7"/>
-      <c r="L194" s="9"/>
+      <c r="N193" s="9"/>
+    </row>
+    <row r="194" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J194" s="80"/>
+      <c r="L194" s="7"/>
       <c r="M194" s="9"/>
-    </row>
-    <row r="195" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I195" s="80"/>
-      <c r="K195" s="7"/>
-      <c r="L195" s="9"/>
+      <c r="N194" s="9"/>
+    </row>
+    <row r="195" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J195" s="80"/>
+      <c r="L195" s="7"/>
       <c r="M195" s="9"/>
-    </row>
-    <row r="196" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I196" s="80"/>
-      <c r="K196" s="7"/>
-      <c r="L196" s="9"/>
+      <c r="N195" s="9"/>
+    </row>
+    <row r="196" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J196" s="80"/>
+      <c r="L196" s="7"/>
       <c r="M196" s="9"/>
-    </row>
-    <row r="197" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I197" s="80"/>
-      <c r="K197" s="7"/>
-      <c r="L197" s="9"/>
+      <c r="N196" s="9"/>
+    </row>
+    <row r="197" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J197" s="80"/>
+      <c r="L197" s="7"/>
       <c r="M197" s="9"/>
-    </row>
-    <row r="198" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I198" s="80"/>
-      <c r="K198" s="7"/>
-      <c r="L198" s="9"/>
+      <c r="N197" s="9"/>
+    </row>
+    <row r="198" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J198" s="80"/>
+      <c r="L198" s="7"/>
       <c r="M198" s="9"/>
-    </row>
-    <row r="199" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I199" s="80"/>
-      <c r="K199" s="7"/>
-      <c r="L199" s="9"/>
+      <c r="N198" s="9"/>
+    </row>
+    <row r="199" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J199" s="80"/>
+      <c r="L199" s="7"/>
       <c r="M199" s="9"/>
-    </row>
-    <row r="200" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I200" s="80"/>
-      <c r="K200" s="7"/>
-      <c r="L200" s="9"/>
+      <c r="N199" s="9"/>
+    </row>
+    <row r="200" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J200" s="80"/>
+      <c r="L200" s="7"/>
       <c r="M200" s="9"/>
-    </row>
-    <row r="201" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I201" s="80"/>
-      <c r="K201" s="7"/>
-      <c r="L201" s="9"/>
+      <c r="N200" s="9"/>
+    </row>
+    <row r="201" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J201" s="80"/>
+      <c r="L201" s="7"/>
       <c r="M201" s="9"/>
-    </row>
-    <row r="202" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I202" s="80"/>
-      <c r="K202" s="7"/>
-      <c r="L202" s="9"/>
+      <c r="N201" s="9"/>
+    </row>
+    <row r="202" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J202" s="80"/>
+      <c r="L202" s="7"/>
       <c r="M202" s="9"/>
-    </row>
-    <row r="203" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I203" s="80"/>
-      <c r="K203" s="7"/>
-      <c r="L203" s="9"/>
+      <c r="N202" s="9"/>
+    </row>
+    <row r="203" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J203" s="80"/>
+      <c r="L203" s="7"/>
       <c r="M203" s="9"/>
-    </row>
-    <row r="204" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I204" s="80"/>
-      <c r="K204" s="7"/>
-      <c r="L204" s="9"/>
+      <c r="N203" s="9"/>
+    </row>
+    <row r="204" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J204" s="80"/>
+      <c r="L204" s="7"/>
       <c r="M204" s="9"/>
-    </row>
-    <row r="205" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I205" s="80"/>
-      <c r="K205" s="7"/>
-      <c r="L205" s="9"/>
+      <c r="N204" s="9"/>
+    </row>
+    <row r="205" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J205" s="80"/>
+      <c r="L205" s="7"/>
       <c r="M205" s="9"/>
-    </row>
-    <row r="206" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I206" s="80"/>
-      <c r="K206" s="7"/>
-      <c r="L206" s="9"/>
+      <c r="N205" s="9"/>
+    </row>
+    <row r="206" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J206" s="80"/>
+      <c r="L206" s="7"/>
       <c r="M206" s="9"/>
-    </row>
-    <row r="207" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I207" s="80"/>
-      <c r="K207" s="7"/>
-      <c r="L207" s="9"/>
+      <c r="N206" s="9"/>
+    </row>
+    <row r="207" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J207" s="80"/>
+      <c r="L207" s="7"/>
       <c r="M207" s="9"/>
-    </row>
-    <row r="208" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I208" s="80"/>
-      <c r="K208" s="7"/>
-      <c r="L208" s="9"/>
+      <c r="N207" s="9"/>
+    </row>
+    <row r="208" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J208" s="80"/>
+      <c r="L208" s="7"/>
       <c r="M208" s="9"/>
-    </row>
-    <row r="209" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I209" s="80"/>
-      <c r="K209" s="7"/>
-      <c r="L209" s="9"/>
+      <c r="N208" s="9"/>
+    </row>
+    <row r="209" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J209" s="80"/>
+      <c r="L209" s="7"/>
       <c r="M209" s="9"/>
-    </row>
-    <row r="210" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I210" s="80"/>
-      <c r="K210" s="7"/>
-      <c r="L210" s="9"/>
+      <c r="N209" s="9"/>
+    </row>
+    <row r="210" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J210" s="80"/>
+      <c r="L210" s="7"/>
       <c r="M210" s="9"/>
-    </row>
-    <row r="211" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I211" s="80"/>
-      <c r="K211" s="7"/>
-      <c r="L211" s="9"/>
+      <c r="N210" s="9"/>
+    </row>
+    <row r="211" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J211" s="80"/>
+      <c r="L211" s="7"/>
       <c r="M211" s="9"/>
-    </row>
-    <row r="212" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I212" s="80"/>
-      <c r="K212" s="7"/>
-      <c r="L212" s="9"/>
+      <c r="N211" s="9"/>
+    </row>
+    <row r="212" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J212" s="80"/>
+      <c r="L212" s="7"/>
       <c r="M212" s="9"/>
-    </row>
-    <row r="213" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I213" s="80"/>
-      <c r="K213" s="7"/>
-      <c r="L213" s="9"/>
+      <c r="N212" s="9"/>
+    </row>
+    <row r="213" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J213" s="80"/>
+      <c r="L213" s="7"/>
       <c r="M213" s="9"/>
-    </row>
-    <row r="214" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I214" s="80"/>
-      <c r="K214" s="7"/>
-      <c r="L214" s="9"/>
+      <c r="N213" s="9"/>
+    </row>
+    <row r="214" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J214" s="80"/>
+      <c r="L214" s="7"/>
       <c r="M214" s="9"/>
-    </row>
-    <row r="215" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I215" s="80"/>
-      <c r="K215" s="7"/>
-      <c r="L215" s="9"/>
+      <c r="N214" s="9"/>
+    </row>
+    <row r="215" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J215" s="80"/>
+      <c r="L215" s="7"/>
       <c r="M215" s="9"/>
-    </row>
-    <row r="216" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I216" s="80"/>
-      <c r="K216" s="7"/>
-      <c r="L216" s="9"/>
+      <c r="N215" s="9"/>
+    </row>
+    <row r="216" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J216" s="80"/>
+      <c r="L216" s="7"/>
       <c r="M216" s="9"/>
-    </row>
-    <row r="217" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I217" s="80"/>
-      <c r="K217" s="7"/>
-      <c r="L217" s="9"/>
+      <c r="N216" s="9"/>
+    </row>
+    <row r="217" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J217" s="80"/>
+      <c r="L217" s="7"/>
       <c r="M217" s="9"/>
-    </row>
-    <row r="218" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I218" s="80"/>
-      <c r="K218" s="7"/>
-      <c r="L218" s="9"/>
+      <c r="N217" s="9"/>
+    </row>
+    <row r="218" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J218" s="80"/>
+      <c r="L218" s="7"/>
       <c r="M218" s="9"/>
-    </row>
-    <row r="219" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I219" s="80"/>
-      <c r="K219" s="7"/>
-      <c r="L219" s="9"/>
+      <c r="N218" s="9"/>
+    </row>
+    <row r="219" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J219" s="80"/>
+      <c r="L219" s="7"/>
       <c r="M219" s="9"/>
-    </row>
-    <row r="220" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I220" s="80"/>
-      <c r="K220" s="7"/>
-      <c r="L220" s="9"/>
+      <c r="N219" s="9"/>
+    </row>
+    <row r="220" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J220" s="80"/>
+      <c r="L220" s="7"/>
       <c r="M220" s="9"/>
-    </row>
-    <row r="221" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I221" s="80"/>
-      <c r="K221" s="7"/>
-      <c r="L221" s="9"/>
+      <c r="N220" s="9"/>
+    </row>
+    <row r="221" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J221" s="80"/>
+      <c r="L221" s="7"/>
       <c r="M221" s="9"/>
-    </row>
-    <row r="222" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I222" s="80"/>
-      <c r="K222" s="7"/>
-      <c r="L222" s="9"/>
+      <c r="N221" s="9"/>
+    </row>
+    <row r="222" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J222" s="80"/>
+      <c r="L222" s="7"/>
       <c r="M222" s="9"/>
-    </row>
-    <row r="223" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I223" s="80"/>
-      <c r="K223" s="7"/>
-      <c r="L223" s="9"/>
+      <c r="N222" s="9"/>
+    </row>
+    <row r="223" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J223" s="80"/>
+      <c r="L223" s="7"/>
       <c r="M223" s="9"/>
-    </row>
-    <row r="224" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I224" s="80"/>
-      <c r="K224" s="7"/>
-      <c r="L224" s="9"/>
+      <c r="N223" s="9"/>
+    </row>
+    <row r="224" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J224" s="80"/>
+      <c r="L224" s="7"/>
       <c r="M224" s="9"/>
-    </row>
-    <row r="225" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I225" s="80"/>
-      <c r="K225" s="7"/>
-      <c r="L225" s="9"/>
+      <c r="N224" s="9"/>
+    </row>
+    <row r="225" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J225" s="80"/>
+      <c r="L225" s="7"/>
       <c r="M225" s="9"/>
-    </row>
-    <row r="226" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I226" s="80"/>
-      <c r="K226" s="7"/>
-      <c r="L226" s="9"/>
+      <c r="N225" s="9"/>
+    </row>
+    <row r="226" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J226" s="80"/>
+      <c r="L226" s="7"/>
       <c r="M226" s="9"/>
-    </row>
-    <row r="227" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I227" s="80"/>
-      <c r="K227" s="7"/>
-      <c r="L227" s="9"/>
+      <c r="N226" s="9"/>
+    </row>
+    <row r="227" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J227" s="80"/>
+      <c r="L227" s="7"/>
       <c r="M227" s="9"/>
-    </row>
-    <row r="228" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I228" s="80"/>
-      <c r="K228" s="7"/>
-      <c r="L228" s="9"/>
+      <c r="N227" s="9"/>
+    </row>
+    <row r="228" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J228" s="80"/>
+      <c r="L228" s="7"/>
       <c r="M228" s="9"/>
-    </row>
-    <row r="229" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I229" s="80"/>
-      <c r="K229" s="7"/>
-      <c r="L229" s="9"/>
+      <c r="N228" s="9"/>
+    </row>
+    <row r="229" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J229" s="80"/>
+      <c r="L229" s="7"/>
       <c r="M229" s="9"/>
-    </row>
-    <row r="230" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I230" s="80"/>
-      <c r="K230" s="7"/>
-      <c r="L230" s="9"/>
+      <c r="N229" s="9"/>
+    </row>
+    <row r="230" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J230" s="80"/>
+      <c r="L230" s="7"/>
       <c r="M230" s="9"/>
-    </row>
-    <row r="231" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I231" s="80"/>
-      <c r="K231" s="7"/>
-      <c r="L231" s="9"/>
+      <c r="N230" s="9"/>
+    </row>
+    <row r="231" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J231" s="80"/>
+      <c r="L231" s="7"/>
       <c r="M231" s="9"/>
-    </row>
-    <row r="232" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I232" s="80"/>
-      <c r="K232" s="7"/>
-      <c r="L232" s="9"/>
+      <c r="N231" s="9"/>
+    </row>
+    <row r="232" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J232" s="80"/>
+      <c r="L232" s="7"/>
       <c r="M232" s="9"/>
-    </row>
-    <row r="233" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I233" s="80"/>
-      <c r="K233" s="7"/>
-      <c r="L233" s="9"/>
+      <c r="N232" s="9"/>
+    </row>
+    <row r="233" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J233" s="80"/>
+      <c r="L233" s="7"/>
       <c r="M233" s="9"/>
-    </row>
-    <row r="234" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I234" s="80"/>
-      <c r="K234" s="7"/>
-      <c r="L234" s="9"/>
+      <c r="N233" s="9"/>
+    </row>
+    <row r="234" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J234" s="80"/>
+      <c r="L234" s="7"/>
       <c r="M234" s="9"/>
-    </row>
-    <row r="235" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I235" s="80"/>
-      <c r="K235" s="7"/>
-      <c r="L235" s="9"/>
+      <c r="N234" s="9"/>
+    </row>
+    <row r="235" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J235" s="80"/>
+      <c r="L235" s="7"/>
       <c r="M235" s="9"/>
-    </row>
-    <row r="236" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I236" s="80"/>
-      <c r="K236" s="7"/>
-      <c r="L236" s="9"/>
+      <c r="N235" s="9"/>
+    </row>
+    <row r="236" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J236" s="80"/>
+      <c r="L236" s="7"/>
       <c r="M236" s="9"/>
-    </row>
-    <row r="237" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I237" s="80"/>
-      <c r="K237" s="7"/>
-      <c r="L237" s="9"/>
+      <c r="N236" s="9"/>
+    </row>
+    <row r="237" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J237" s="80"/>
+      <c r="L237" s="7"/>
       <c r="M237" s="9"/>
-    </row>
-    <row r="238" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I238" s="80"/>
-      <c r="K238" s="7"/>
-      <c r="L238" s="9"/>
+      <c r="N237" s="9"/>
+    </row>
+    <row r="238" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J238" s="80"/>
+      <c r="L238" s="7"/>
       <c r="M238" s="9"/>
-    </row>
-    <row r="239" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I239" s="80"/>
-      <c r="K239" s="7"/>
-      <c r="L239" s="9"/>
+      <c r="N238" s="9"/>
+    </row>
+    <row r="239" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J239" s="80"/>
+      <c r="L239" s="7"/>
       <c r="M239" s="9"/>
-    </row>
-    <row r="240" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I240" s="80"/>
-      <c r="K240" s="7"/>
-      <c r="L240" s="9"/>
+      <c r="N239" s="9"/>
+    </row>
+    <row r="240" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J240" s="80"/>
+      <c r="L240" s="7"/>
       <c r="M240" s="9"/>
-    </row>
-    <row r="241" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I241" s="80"/>
-      <c r="K241" s="7"/>
-      <c r="L241" s="9"/>
+      <c r="N240" s="9"/>
+    </row>
+    <row r="241" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J241" s="80"/>
+      <c r="L241" s="7"/>
       <c r="M241" s="9"/>
-    </row>
-    <row r="242" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I242" s="80"/>
-      <c r="K242" s="7"/>
-      <c r="L242" s="9"/>
+      <c r="N241" s="9"/>
+    </row>
+    <row r="242" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J242" s="80"/>
+      <c r="L242" s="7"/>
       <c r="M242" s="9"/>
-    </row>
-    <row r="243" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I243" s="80"/>
-      <c r="K243" s="7"/>
-      <c r="L243" s="9"/>
+      <c r="N242" s="9"/>
+    </row>
+    <row r="243" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J243" s="80"/>
+      <c r="L243" s="7"/>
       <c r="M243" s="9"/>
-    </row>
-    <row r="244" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I244" s="80"/>
-      <c r="K244" s="7"/>
-      <c r="L244" s="9"/>
+      <c r="N243" s="9"/>
+    </row>
+    <row r="244" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J244" s="80"/>
+      <c r="L244" s="7"/>
       <c r="M244" s="9"/>
-    </row>
-    <row r="245" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I245" s="80"/>
-      <c r="K245" s="7"/>
-      <c r="L245" s="9"/>
+      <c r="N244" s="9"/>
+    </row>
+    <row r="245" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J245" s="80"/>
+      <c r="L245" s="7"/>
       <c r="M245" s="9"/>
-    </row>
-    <row r="246" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I246" s="80"/>
-      <c r="K246" s="7"/>
-      <c r="L246" s="9"/>
+      <c r="N245" s="9"/>
+    </row>
+    <row r="246" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J246" s="80"/>
+      <c r="L246" s="7"/>
       <c r="M246" s="9"/>
-    </row>
-    <row r="247" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I247" s="80"/>
-      <c r="K247" s="7"/>
-      <c r="L247" s="9"/>
+      <c r="N246" s="9"/>
+    </row>
+    <row r="247" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J247" s="80"/>
+      <c r="L247" s="7"/>
       <c r="M247" s="9"/>
-    </row>
-    <row r="248" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I248" s="80"/>
-      <c r="K248" s="7"/>
-      <c r="L248" s="9"/>
+      <c r="N247" s="9"/>
+    </row>
+    <row r="248" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J248" s="80"/>
+      <c r="L248" s="7"/>
       <c r="M248" s="9"/>
-    </row>
-    <row r="249" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I249" s="80"/>
-      <c r="K249" s="7"/>
-      <c r="L249" s="9"/>
+      <c r="N248" s="9"/>
+    </row>
+    <row r="249" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J249" s="80"/>
+      <c r="L249" s="7"/>
       <c r="M249" s="9"/>
-    </row>
-    <row r="250" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I250" s="80"/>
-      <c r="K250" s="7"/>
-      <c r="L250" s="9"/>
+      <c r="N249" s="9"/>
+    </row>
+    <row r="250" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J250" s="80"/>
+      <c r="L250" s="7"/>
       <c r="M250" s="9"/>
-    </row>
-    <row r="251" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I251" s="80"/>
-      <c r="K251" s="7"/>
-      <c r="L251" s="9"/>
+      <c r="N250" s="9"/>
+    </row>
+    <row r="251" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J251" s="80"/>
+      <c r="L251" s="7"/>
       <c r="M251" s="9"/>
-    </row>
-    <row r="252" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I252" s="80"/>
-      <c r="K252" s="7"/>
-      <c r="L252" s="9"/>
+      <c r="N251" s="9"/>
+    </row>
+    <row r="252" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J252" s="80"/>
+      <c r="L252" s="7"/>
       <c r="M252" s="9"/>
-    </row>
-    <row r="253" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I253" s="80"/>
-      <c r="K253" s="7"/>
-      <c r="L253" s="9"/>
+      <c r="N252" s="9"/>
+    </row>
+    <row r="253" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J253" s="80"/>
+      <c r="L253" s="7"/>
       <c r="M253" s="9"/>
+      <c r="N253" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K8:K253">
+  <conditionalFormatting sqref="L8:L253">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4242,7 +4387,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
+  <conditionalFormatting sqref="J1:J1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4277,10 +4422,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="B3:O27"/>
+  <dimension ref="B3:O28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4312,7 +4457,7 @@
       </c>
       <c r="G3" s="95">
         <f ca="1">TODAY()</f>
-        <v>43257</v>
+        <v>43258</v>
       </c>
       <c r="H3" s="117" t="s">
         <v>74</v>
@@ -4325,7 +4470,7 @@
       </c>
       <c r="L3" s="95">
         <f ca="1">TODAY()+1</f>
-        <v>43258</v>
+        <v>43259</v>
       </c>
       <c r="M3" s="117" t="s">
         <v>74</v>
@@ -4351,7 +4496,7 @@
       <c r="N4" s="94"/>
       <c r="O4" s="99"/>
     </row>
-    <row r="5" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="107" t="s">
         <v>151</v>
       </c>
@@ -4362,8 +4507,12 @@
       <c r="E5" s="109">
         <v>1</v>
       </c>
-      <c r="G5" s="100"/>
-      <c r="H5" s="43"/>
+      <c r="G5" s="100" t="s">
+        <v>175</v>
+      </c>
+      <c r="H5" s="43" t="s">
+        <v>176</v>
+      </c>
       <c r="I5" s="43"/>
       <c r="J5" s="101"/>
       <c r="L5" s="100"/>
@@ -4442,7 +4591,7 @@
         <v>0.2</v>
       </c>
       <c r="E9" s="109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="100"/>
       <c r="H9" s="43"/>
@@ -4462,7 +4611,7 @@
         <v>0.5</v>
       </c>
       <c r="E10" s="109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="100"/>
       <c r="H10" s="43"/>
@@ -4484,7 +4633,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="100"/>
       <c r="H11" s="43"/>
@@ -4495,15 +4644,15 @@
       <c r="N11" s="43"/>
       <c r="O11" s="101"/>
     </row>
-    <row r="12" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="113"/>
-      <c r="C12" s="116" t="s">
-        <v>158</v>
-      </c>
-      <c r="D12" s="114">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E12" s="115"/>
+    <row r="12" spans="2:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="107" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="108"/>
+      <c r="D12" s="108"/>
+      <c r="E12" s="109">
+        <v>0</v>
+      </c>
       <c r="G12" s="100"/>
       <c r="H12" s="43"/>
       <c r="I12" s="43"/>
@@ -4514,16 +4663,14 @@
       <c r="O12" s="101"/>
     </row>
     <row r="13" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="107" t="s">
-        <v>159</v>
-      </c>
-      <c r="C13" s="108"/>
-      <c r="D13" s="108">
-        <v>0.5</v>
-      </c>
-      <c r="E13" s="109">
-        <v>0</v>
-      </c>
+      <c r="B13" s="113"/>
+      <c r="C13" s="116" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" s="114">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E13" s="115"/>
       <c r="G13" s="100"/>
       <c r="H13" s="43"/>
       <c r="I13" s="43"/>
@@ -4535,11 +4682,11 @@
     </row>
     <row r="14" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="107" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C14" s="108"/>
       <c r="D14" s="108">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E14" s="109">
         <v>0</v>
@@ -4555,7 +4702,7 @@
     </row>
     <row r="15" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="107" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C15" s="108"/>
       <c r="D15" s="108">
@@ -4574,14 +4721,16 @@
       <c r="O15" s="101"/>
     </row>
     <row r="16" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="113"/>
-      <c r="C16" s="116" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="114">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E16" s="115"/>
+      <c r="B16" s="107" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="108"/>
+      <c r="D16" s="108">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="109">
+        <v>0</v>
+      </c>
       <c r="G16" s="100"/>
       <c r="H16" s="43"/>
       <c r="I16" s="43"/>
@@ -4592,10 +4741,14 @@
       <c r="O16" s="101"/>
     </row>
     <row r="17" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="107"/>
-      <c r="C17" s="108"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="109"/>
+      <c r="B17" s="113"/>
+      <c r="C17" s="116" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="114">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E17" s="115"/>
       <c r="G17" s="100"/>
       <c r="H17" s="43"/>
       <c r="I17" s="43"/>
@@ -4732,21 +4885,35 @@
       <c r="O26" s="101"/>
     </row>
     <row r="27" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="110"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="112"/>
-      <c r="G27" s="102"/>
-      <c r="H27" s="103"/>
-      <c r="I27" s="103"/>
-      <c r="J27" s="104"/>
-      <c r="L27" s="102"/>
-      <c r="M27" s="103"/>
-      <c r="N27" s="103"/>
-      <c r="O27" s="104"/>
+      <c r="B27" s="107"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="109"/>
+      <c r="G27" s="100"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="101"/>
+      <c r="L27" s="100"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="101"/>
+    </row>
+    <row r="28" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="110"/>
+      <c r="C28" s="111"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="112"/>
+      <c r="G28" s="102"/>
+      <c r="H28" s="103"/>
+      <c r="I28" s="103"/>
+      <c r="J28" s="104"/>
+      <c r="L28" s="102"/>
+      <c r="M28" s="103"/>
+      <c r="N28" s="103"/>
+      <c r="O28" s="104"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E5:E15 E17:E27">
+  <conditionalFormatting sqref="E5:E16 E18:E28">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4758,7 +4925,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O5:O27">
+  <conditionalFormatting sqref="O5:O28">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4770,7 +4937,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5:J27">
+  <conditionalFormatting sqref="J5:J28">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4782,7 +4949,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
+  <conditionalFormatting sqref="E17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4803,8 +4970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K370"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A16" zoomScale="106" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9693,12 +9860,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:G369">
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>INDIRECT("B"&amp;ROW())=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:B369">
-    <cfRule type="timePeriod" dxfId="12" priority="1" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="today">
       <formula>FLOOR(B9,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9749,7 +9916,7 @@
       </c>
       <c r="E4" s="11">
         <f ca="1">TODAY()</f>
-        <v>43257</v>
+        <v>43258</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
IK Bone (Almost Done)
</commit_message>
<xml_diff>
--- a/Management & Logging/Planning and Management/AgilePlanning.xlsx
+++ b/Management & Logging/Planning and Management/AgilePlanning.xlsx
@@ -1398,7 +1398,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1757,6 +1757,9 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="27" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="7" fillId="10" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1770,6 +1773,41 @@
     <cellStyle name="Style 1" xfId="1"/>
   </cellStyles>
   <dxfs count="28">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1813,45 +1851,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1906,33 +1909,33 @@
     <tableColumn id="4" name="BT 0.2" dataDxfId="22"/>
     <tableColumn id="5" name="BT 0.3" dataDxfId="21"/>
     <tableColumn id="6" name="Break Down Notes" dataDxfId="20"/>
-    <tableColumn id="12" name="Issues/Notes" dataDxfId="0"/>
-    <tableColumn id="11" name="Hours left" dataDxfId="19">
+    <tableColumn id="12" name="Issues/Notes" dataDxfId="19"/>
+    <tableColumn id="11" name="Hours left" dataDxfId="18">
       <calculatedColumnFormula>_xlfn.DAYS(TODAY(), M8)*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Completion Hours" dataDxfId="18"/>
-    <tableColumn id="8" name="Current Progress" dataDxfId="17"/>
-    <tableColumn id="9" name="Expected Completion Date" dataDxfId="16"/>
-    <tableColumn id="10" name="Real Completion Date" dataDxfId="15"/>
+    <tableColumn id="7" name="Completion Hours" dataDxfId="17"/>
+    <tableColumn id="8" name="Current Progress" dataDxfId="16"/>
+    <tableColumn id="9" name="Expected Completion Date" dataDxfId="15"/>
+    <tableColumn id="10" name="Real Completion Date" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="C7:L233" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="C7:L233" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="C7:L233"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="REF TAG" dataDxfId="12"/>
-    <tableColumn id="2" name="Task Name" dataDxfId="11"/>
-    <tableColumn id="3" name="BT 0.1" dataDxfId="10"/>
-    <tableColumn id="4" name="BT 0.2" dataDxfId="9"/>
-    <tableColumn id="5" name="BT 0.3" dataDxfId="8"/>
-    <tableColumn id="6" name="Break Down Notes" dataDxfId="7"/>
-    <tableColumn id="7" name="Completion Hours" dataDxfId="6"/>
-    <tableColumn id="8" name="Current Progress" dataDxfId="5"/>
-    <tableColumn id="9" name="Expected Completion Date" dataDxfId="4"/>
-    <tableColumn id="10" name="Real Completion Date" dataDxfId="3"/>
+    <tableColumn id="1" name="REF TAG" dataDxfId="9"/>
+    <tableColumn id="2" name="Task Name" dataDxfId="8"/>
+    <tableColumn id="3" name="BT 0.1" dataDxfId="7"/>
+    <tableColumn id="4" name="BT 0.2" dataDxfId="6"/>
+    <tableColumn id="5" name="BT 0.3" dataDxfId="5"/>
+    <tableColumn id="6" name="Break Down Notes" dataDxfId="4"/>
+    <tableColumn id="7" name="Completion Hours" dataDxfId="3"/>
+    <tableColumn id="8" name="Current Progress" dataDxfId="2"/>
+    <tableColumn id="9" name="Expected Completion Date" dataDxfId="1"/>
+    <tableColumn id="10" name="Real Completion Date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2206,8 +2209,8 @@
   </sheetPr>
   <dimension ref="A1:N253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="97" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2237,7 +2240,7 @@
       </c>
       <c r="E4" s="11">
         <f ca="1">TODAY()</f>
-        <v>43258</v>
+        <v>43266</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>10</v>
@@ -2315,7 +2318,7 @@
       </c>
       <c r="J8" s="80">
         <f ca="1">ABS(_xlfn.DAYS(TODAY(), M8)*24)</f>
-        <v>528</v>
+        <v>720</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>18</v>
@@ -2394,7 +2397,7 @@
       </c>
       <c r="J14" s="80">
         <f ca="1">ABS(_xlfn.DAYS(TODAY(), M14)*24)</f>
-        <v>48</v>
+        <v>240</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>27</v>
@@ -2500,7 +2503,7 @@
       </c>
       <c r="J22" s="80">
         <f ca="1">ABS(_xlfn.DAYS(TODAY(), M22)*24)</f>
-        <v>360</v>
+        <v>552</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>64</v>
@@ -2644,7 +2647,7 @@
       </c>
       <c r="J33" s="80">
         <f ca="1">ABS(_xlfn.DAYS(TODAY(), M33)*24)</f>
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>65</v>
@@ -2834,7 +2837,7 @@
       <c r="E47" s="14"/>
       <c r="J47" s="80">
         <f ca="1">ABS(_xlfn.DAYS(TODAY(), M47)*24)</f>
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="K47" s="1">
         <v>50</v>
@@ -2871,14 +2874,14 @@
         <v>180</v>
       </c>
       <c r="J49" s="80">
-        <f t="shared" ref="J48:J55" ca="1" si="0">ABS(_xlfn.DAYS(TODAY(), M49)*24)</f>
-        <v>192</v>
+        <f t="shared" ref="J49:J55" ca="1" si="0">ABS(_xlfn.DAYS(TODAY(), M49)*24)</f>
+        <v>360</v>
       </c>
       <c r="L49" s="7">
         <v>0</v>
       </c>
       <c r="M49" s="9">
-        <v>43266</v>
+        <v>43281</v>
       </c>
       <c r="N49" s="9"/>
     </row>
@@ -2900,14 +2903,14 @@
         <v>179</v>
       </c>
       <c r="J50" s="80">
-        <f t="shared" ca="1" si="0"/>
-        <v>120</v>
+        <f ca="1">ABS(_xlfn.DAYS(TODAY(), M50)*24)</f>
+        <v>240</v>
       </c>
       <c r="L50" s="7">
         <v>0.75</v>
       </c>
       <c r="M50" s="9">
-        <v>43263</v>
+        <v>43276</v>
       </c>
       <c r="N50" s="9"/>
     </row>
@@ -2933,13 +2936,13 @@
       </c>
       <c r="J51" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>120</v>
+        <v>264</v>
       </c>
       <c r="L51" s="7">
         <v>0.75</v>
       </c>
       <c r="M51" s="9">
-        <v>43263</v>
+        <v>43277</v>
       </c>
       <c r="N51" s="9"/>
     </row>
@@ -2962,13 +2965,13 @@
       </c>
       <c r="J52" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>120</v>
+        <v>288</v>
       </c>
       <c r="L52" s="7">
         <v>0</v>
       </c>
       <c r="M52" s="9">
-        <v>43263</v>
+        <v>43278</v>
       </c>
       <c r="N52" s="9"/>
     </row>
@@ -2988,13 +2991,13 @@
       </c>
       <c r="J53" s="80">
         <f t="shared" ca="1" si="0"/>
-        <v>120</v>
+        <v>1584</v>
       </c>
       <c r="L53" s="7">
         <v>0</v>
       </c>
       <c r="M53" s="9">
-        <v>43263</v>
+        <v>43200</v>
       </c>
       <c r="N53" s="9"/>
     </row>
@@ -3010,19 +3013,23 @@
     </row>
     <row r="55" spans="3:14" ht="60" x14ac:dyDescent="0.25">
       <c r="C55" s="92"/>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="14"/>
-      <c r="I55" s="1" t="s">
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="30"/>
+      <c r="I55" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="J55" s="80">
+      <c r="J55" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="L55" s="7"/>
-      <c r="M55" s="9">
+        <v>72</v>
+      </c>
+      <c r="K55" s="30"/>
+      <c r="L55" s="122"/>
+      <c r="M55" s="29">
         <v>43263</v>
       </c>
       <c r="N55" s="9"/>
@@ -3035,7 +3042,7 @@
       <c r="M56" s="9"/>
       <c r="N56" s="9"/>
     </row>
-    <row r="57" spans="3:14" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:14" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E57" s="14"/>
       <c r="H57" s="121" t="s">
         <v>185</v>
@@ -3062,7 +3069,7 @@
       </c>
       <c r="J59" s="80">
         <f ca="1">ABS(_xlfn.DAYS(TODAY(), M59)*24)</f>
-        <v>1608</v>
+        <v>1800</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>66</v>
@@ -4457,7 +4464,7 @@
       </c>
       <c r="G3" s="95">
         <f ca="1">TODAY()</f>
-        <v>43258</v>
+        <v>43266</v>
       </c>
       <c r="H3" s="117" t="s">
         <v>74</v>
@@ -4470,7 +4477,7 @@
       </c>
       <c r="L3" s="95">
         <f ca="1">TODAY()+1</f>
-        <v>43259</v>
+        <v>43267</v>
       </c>
       <c r="M3" s="117" t="s">
         <v>74</v>
@@ -9860,12 +9867,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:G369">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>INDIRECT("B"&amp;ROW())=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:B369">
-    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="12" priority="1" timePeriod="today">
       <formula>FLOOR(B9,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9916,7 +9923,7 @@
       </c>
       <c r="E4" s="11">
         <f ca="1">TODAY()</f>
-        <v>43258</v>
+        <v>43266</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>10</v>

</xml_diff>